<commit_message>
adicionando dados das imagens ao desenvolvimento
</commit_message>
<xml_diff>
--- a/resultados/resultados.xlsx
+++ b/resultados/resultados.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Berea200" sheetId="1" state="visible" r:id="rId1"/>
@@ -67,94 +67,94 @@
     <t xml:space="preserve">I31 </t>
   </si>
   <si>
+    <t xml:space="preserve">3271i01 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3271i02 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3271i03 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3271i04 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3271i05 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3271i06 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3271i07 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3271i08 </t>
+  </si>
+  <si>
     <t xml:space="preserve">3271i09 </t>
   </si>
   <si>
-    <t xml:space="preserve">3271i02 </t>
-  </si>
-  <si>
     <t xml:space="preserve">3271i10 </t>
   </si>
   <si>
-    <t xml:space="preserve">3271i01 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3271i04 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3271i07 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3271i05 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3271i03 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3271i08 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3271i06 </t>
+    <t xml:space="preserve">3251i01 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3251i02 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3251i03 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3251i04 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3251i05 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3251i06 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3251i07 </t>
   </si>
   <si>
     <t xml:space="preserve">3251i08 </t>
   </si>
   <si>
-    <t xml:space="preserve">3251i02 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3251i05 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3251i06 </t>
-  </si>
-  <si>
     <t xml:space="preserve">3251i09 </t>
   </si>
   <si>
-    <t xml:space="preserve">3251i07 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3251i03 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3251i04 </t>
-  </si>
-  <si>
     <t xml:space="preserve">3251i10 </t>
   </si>
   <si>
-    <t xml:space="preserve">3251i01 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">L67409i5 </t>
+    <t xml:space="preserve">L67409i01 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L67409i02 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L67409i03 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L67409i04 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L67409i05 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L67409i06 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L67409i07 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L67409i08 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L67409i09 </t>
   </si>
   <si>
     <t xml:space="preserve">L67409i10 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">L67409i1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">L67409i8 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">L67409i3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">L67409i2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">L67409i7 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">L67409i6 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">L67409i4 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">L67409i9 </t>
   </si>
 </sst>
 </file>
@@ -201,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1"/>
@@ -210,6 +210,9 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="161" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="162" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -1046,16 +1049,16 @@
         <v>16</v>
       </c>
       <c r="B2">
-        <v>0.22583658854166666</v>
+        <v>0.24501953125000001</v>
       </c>
       <c r="C2">
-        <v>19.478908061981201</v>
+        <v>20.62668776512146</v>
       </c>
       <c r="D2">
-        <v>1646</v>
+        <v>1210</v>
       </c>
       <c r="E2">
-        <v>2137</v>
+        <v>2382</v>
       </c>
     </row>
     <row r="3" ht="14.25">
@@ -1080,16 +1083,16 @@
         <v>18</v>
       </c>
       <c r="B4">
-        <v>0.27026041666666667</v>
+        <v>0.20591471354166666</v>
       </c>
       <c r="C4">
-        <v>20.704411745071411</v>
+        <v>20.686766862869263</v>
       </c>
       <c r="D4">
-        <v>1179</v>
+        <v>1733</v>
       </c>
       <c r="E4">
-        <v>2052</v>
+        <v>2557</v>
       </c>
     </row>
     <row r="5" ht="14.25">
@@ -1097,16 +1100,16 @@
         <v>19</v>
       </c>
       <c r="B5">
-        <v>0.24501953125000001</v>
+        <v>0.093710937499999994</v>
       </c>
       <c r="C5">
-        <v>20.62668776512146</v>
+        <v>20.822933435440063</v>
       </c>
       <c r="D5">
-        <v>1210</v>
+        <v>1342</v>
       </c>
       <c r="E5">
-        <v>2382</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="6" ht="14.25">
@@ -1114,16 +1117,16 @@
         <v>20</v>
       </c>
       <c r="B6">
-        <v>0.093710937499999994</v>
+        <v>0.24616536458333332</v>
       </c>
       <c r="C6">
-        <v>20.822933435440063</v>
+        <v>20.532556056976318</v>
       </c>
       <c r="D6">
-        <v>1342</v>
+        <v>1541</v>
       </c>
       <c r="E6">
-        <v>2113</v>
+        <v>2279</v>
       </c>
     </row>
     <row r="7" ht="14.25">
@@ -1131,16 +1134,16 @@
         <v>21</v>
       </c>
       <c r="B7">
-        <v>0.30426757812499999</v>
+        <v>0.37842447916666666</v>
       </c>
       <c r="C7">
-        <v>20.724771976470947</v>
+        <v>20.930784940719604</v>
       </c>
       <c r="D7">
-        <v>1386</v>
+        <v>1377</v>
       </c>
       <c r="E7">
-        <v>2544</v>
+        <v>1765</v>
       </c>
     </row>
     <row r="8" ht="14.25">
@@ -1148,16 +1151,16 @@
         <v>22</v>
       </c>
       <c r="B8">
-        <v>0.24616536458333332</v>
+        <v>0.30426757812499999</v>
       </c>
       <c r="C8">
-        <v>20.532556056976318</v>
+        <v>20.724771976470947</v>
       </c>
       <c r="D8">
-        <v>1541</v>
+        <v>1386</v>
       </c>
       <c r="E8">
-        <v>2279</v>
+        <v>2544</v>
       </c>
     </row>
     <row r="9" ht="14.25">
@@ -1165,16 +1168,16 @@
         <v>23</v>
       </c>
       <c r="B9">
-        <v>0.20591471354166666</v>
+        <v>0.33873046875000001</v>
       </c>
       <c r="C9">
-        <v>20.686766862869263</v>
+        <v>20.581314325332642</v>
       </c>
       <c r="D9">
-        <v>1733</v>
+        <v>1484</v>
       </c>
       <c r="E9">
-        <v>2557</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="10" ht="14.25">
@@ -1182,16 +1185,16 @@
         <v>24</v>
       </c>
       <c r="B10">
-        <v>0.33873046875000001</v>
+        <v>0.22583658854166666</v>
       </c>
       <c r="C10">
-        <v>20.581314325332642</v>
+        <v>19.478908061981201</v>
       </c>
       <c r="D10">
-        <v>1484</v>
+        <v>1646</v>
       </c>
       <c r="E10">
-        <v>1629</v>
+        <v>2137</v>
       </c>
     </row>
     <row r="11" ht="14.25">
@@ -1199,19 +1202,22 @@
         <v>25</v>
       </c>
       <c r="B11">
-        <v>0.37842447916666666</v>
+        <v>0.27026041666666667</v>
       </c>
       <c r="C11">
-        <v>20.930784940719604</v>
+        <v>20.704411745071411</v>
       </c>
       <c r="D11">
-        <v>1377</v>
+        <v>1179</v>
       </c>
       <c r="E11">
-        <v>1765</v>
+        <v>2052</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:E11" columnSort="0">
+    <sortCondition sortBy="value" descending="0" ref="A2:A11"/>
+  </sortState>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157500000008" bottom="0.78740157500000008" header="0.31496062000000014" footer="0.31496062000000014"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
@@ -1259,16 +1265,16 @@
         <v>26</v>
       </c>
       <c r="B2" s="8">
-        <v>0.35732421874999998</v>
+        <v>0.27605794270833334</v>
       </c>
       <c r="C2" s="8">
-        <v>19.931941032409668</v>
+        <v>19.107846975326538</v>
       </c>
       <c r="D2" s="8">
-        <v>2294</v>
+        <v>1906</v>
       </c>
       <c r="E2" s="8">
-        <v>2275</v>
+        <v>2257</v>
       </c>
     </row>
     <row r="3" ht="14.25">
@@ -1293,16 +1299,16 @@
         <v>28</v>
       </c>
       <c r="B4" s="8">
-        <v>0.25666666666666665</v>
+        <v>0.27746744791666667</v>
       </c>
       <c r="C4" s="8">
-        <v>19.21749210357666</v>
+        <v>19.24512243270874</v>
       </c>
       <c r="D4" s="8">
-        <v>2033</v>
+        <v>2651</v>
       </c>
       <c r="E4" s="8">
-        <v>2168</v>
+        <v>2898</v>
       </c>
     </row>
     <row r="5" ht="14.25">
@@ -1310,16 +1316,16 @@
         <v>29</v>
       </c>
       <c r="B5" s="8">
-        <v>0.28517578124999998</v>
+        <v>0.31875976562500002</v>
       </c>
       <c r="C5" s="8">
-        <v>19.658978462219238</v>
+        <v>19.038064241409302</v>
       </c>
       <c r="D5" s="8">
-        <v>2516</v>
+        <v>2220</v>
       </c>
       <c r="E5" s="8">
-        <v>2517</v>
+        <v>3189</v>
       </c>
     </row>
     <row r="6" ht="14.25">
@@ -1327,16 +1333,16 @@
         <v>30</v>
       </c>
       <c r="B6" s="8">
-        <v>0.27944010416666665</v>
+        <v>0.25666666666666665</v>
       </c>
       <c r="C6" s="8">
-        <v>19.275683641433716</v>
+        <v>19.21749210357666</v>
       </c>
       <c r="D6" s="8">
-        <v>2673</v>
+        <v>2033</v>
       </c>
       <c r="E6" s="8">
-        <v>3429</v>
+        <v>2168</v>
       </c>
     </row>
     <row r="7" ht="14.25">
@@ -1344,16 +1350,16 @@
         <v>31</v>
       </c>
       <c r="B7" s="8">
-        <v>0.43480468750000001</v>
+        <v>0.28517578124999998</v>
       </c>
       <c r="C7" s="8">
-        <v>19.249736785888672</v>
+        <v>19.658978462219238</v>
       </c>
       <c r="D7" s="8">
-        <v>2691</v>
+        <v>2516</v>
       </c>
       <c r="E7" s="8">
-        <v>2311</v>
+        <v>2517</v>
       </c>
     </row>
     <row r="8" ht="14.25">
@@ -1361,16 +1367,16 @@
         <v>32</v>
       </c>
       <c r="B8" s="8">
-        <v>0.27746744791666667</v>
+        <v>0.43480468750000001</v>
       </c>
       <c r="C8" s="8">
-        <v>19.24512243270874</v>
+        <v>19.249736785888672</v>
       </c>
       <c r="D8" s="8">
-        <v>2651</v>
+        <v>2691</v>
       </c>
       <c r="E8" s="8">
-        <v>2898</v>
+        <v>2311</v>
       </c>
     </row>
     <row r="9" ht="14.25">
@@ -1378,16 +1384,16 @@
         <v>33</v>
       </c>
       <c r="B9" s="8">
-        <v>0.31875976562500002</v>
+        <v>0.35732421874999998</v>
       </c>
       <c r="C9" s="8">
-        <v>19.038064241409302</v>
+        <v>19.931941032409668</v>
       </c>
       <c r="D9" s="8">
-        <v>2220</v>
+        <v>2294</v>
       </c>
       <c r="E9" s="8">
-        <v>3189</v>
+        <v>2275</v>
       </c>
     </row>
     <row r="10" ht="14.25">
@@ -1395,16 +1401,16 @@
         <v>34</v>
       </c>
       <c r="B10" s="8">
-        <v>0.33397135416666668</v>
+        <v>0.27944010416666665</v>
       </c>
       <c r="C10" s="8">
-        <v>19.238723993301392</v>
+        <v>19.275683641433716</v>
       </c>
       <c r="D10" s="8">
-        <v>2112</v>
+        <v>2673</v>
       </c>
       <c r="E10" s="8">
-        <v>2426</v>
+        <v>3429</v>
       </c>
     </row>
     <row r="11" ht="14.25">
@@ -1412,19 +1418,22 @@
         <v>35</v>
       </c>
       <c r="B11" s="8">
-        <v>0.27605794270833334</v>
+        <v>0.33397135416666668</v>
       </c>
       <c r="C11" s="8">
-        <v>19.107846975326538</v>
+        <v>19.238723993301392</v>
       </c>
       <c r="D11" s="8">
-        <v>1906</v>
+        <v>2112</v>
       </c>
       <c r="E11" s="8">
-        <v>2257</v>
+        <v>2426</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:E11" columnSort="0">
+    <sortCondition sortBy="value" descending="0" ref="A2:A11"/>
+  </sortState>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157500000008" bottom="0.78740157500000008" header="0.31496062000000014" footer="0.31496062000000014"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
@@ -1468,109 +1477,109 @@
       </c>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="8">
+        <v>0.20133789062499999</v>
+      </c>
+      <c r="C2" s="8">
+        <v>21.443613290786743</v>
+      </c>
+      <c r="D2" s="8">
+        <v>3022</v>
+      </c>
+      <c r="E2" s="8">
+        <v>3948</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="A3" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="8">
+        <v>0.19438476562500001</v>
+      </c>
+      <c r="C3" s="8">
+        <v>21.069869041442871</v>
+      </c>
+      <c r="D3" s="8">
+        <v>5921</v>
+      </c>
+      <c r="E3" s="8">
+        <v>6761</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="A4" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="8">
+        <v>0.16281901041666666</v>
+      </c>
+      <c r="C4" s="8">
+        <v>21.49488353729248</v>
+      </c>
+      <c r="D4" s="8">
+        <v>3024</v>
+      </c>
+      <c r="E4" s="8">
+        <v>4209</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="A5" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="8">
+        <v>0.16997721354166667</v>
+      </c>
+      <c r="C5" s="8">
+        <v>20.347252130508423</v>
+      </c>
+      <c r="D5" s="8">
+        <v>1900</v>
+      </c>
+      <c r="E5" s="8">
+        <v>2963</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="A6" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="8">
         <v>0.22072916666666667</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C6" s="8">
         <v>19.879645824432373</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D6" s="8">
         <v>3112</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E6" s="8">
         <v>4529</v>
       </c>
     </row>
-    <row r="3" ht="14.25">
-      <c r="A3" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="8">
-        <v>0.19612630208333334</v>
-      </c>
-      <c r="C3" s="8">
-        <v>21.238434314727783</v>
-      </c>
-      <c r="D3" s="8">
-        <v>3662</v>
-      </c>
-      <c r="E3" s="8">
-        <v>5946</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25">
-      <c r="A4" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="8">
-        <v>0.20133789062499999</v>
-      </c>
-      <c r="C4" s="8">
-        <v>21.443613290786743</v>
-      </c>
-      <c r="D4" s="8">
-        <v>3022</v>
-      </c>
-      <c r="E4" s="8">
-        <v>3948</v>
-      </c>
-    </row>
-    <row r="5" ht="14.25">
-      <c r="A5" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="8">
-        <v>0.10691080729166667</v>
-      </c>
-      <c r="C5" s="8">
-        <v>20.928617477416992</v>
-      </c>
-      <c r="D5" s="8">
-        <v>3181</v>
-      </c>
-      <c r="E5" s="8">
-        <v>5068</v>
-      </c>
-    </row>
-    <row r="6" ht="14.25">
-      <c r="A6" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6" s="8">
-        <v>0.16281901041666666</v>
-      </c>
-      <c r="C6" s="8">
-        <v>21.49488353729248</v>
-      </c>
-      <c r="D6" s="8">
-        <v>3024</v>
-      </c>
-      <c r="E6" s="8">
-        <v>4209</v>
-      </c>
-    </row>
     <row r="7" ht="14.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="9" t="s">
         <v>41</v>
       </c>
       <c r="B7" s="8">
-        <v>0.19438476562500001</v>
+        <v>0.20756510416666665</v>
       </c>
       <c r="C7" s="8">
-        <v>21.069869041442871</v>
+        <v>21.484671592712402</v>
       </c>
       <c r="D7" s="8">
-        <v>5921</v>
+        <v>2154</v>
       </c>
       <c r="E7" s="8">
-        <v>6761</v>
+        <v>3869</v>
       </c>
     </row>
     <row r="8" ht="14.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="9" t="s">
         <v>42</v>
       </c>
       <c r="B8" s="8">
@@ -1587,37 +1596,37 @@
       </c>
     </row>
     <row r="9" ht="14.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="9" t="s">
         <v>43</v>
       </c>
       <c r="B9" s="8">
-        <v>0.20756510416666665</v>
+        <v>0.10691080729166667</v>
       </c>
       <c r="C9" s="8">
-        <v>21.484671592712402</v>
+        <v>20.928617477416992</v>
       </c>
       <c r="D9" s="8">
-        <v>2154</v>
+        <v>3181</v>
       </c>
       <c r="E9" s="8">
-        <v>3869</v>
+        <v>5068</v>
       </c>
     </row>
     <row r="10" ht="14.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="9" t="s">
         <v>44</v>
       </c>
       <c r="B10" s="8">
-        <v>0.16997721354166667</v>
+        <v>0.11185872395833334</v>
       </c>
       <c r="C10" s="8">
-        <v>20.347252130508423</v>
+        <v>21.238481760025024</v>
       </c>
       <c r="D10" s="8">
-        <v>1900</v>
+        <v>2178</v>
       </c>
       <c r="E10" s="8">
-        <v>2963</v>
+        <v>4468</v>
       </c>
     </row>
     <row r="11" ht="14.25">
@@ -1625,19 +1634,22 @@
         <v>45</v>
       </c>
       <c r="B11" s="8">
-        <v>0.11185872395833334</v>
+        <v>0.19612630208333334</v>
       </c>
       <c r="C11" s="8">
-        <v>21.238481760025024</v>
+        <v>21.238434314727783</v>
       </c>
       <c r="D11" s="8">
-        <v>2178</v>
+        <v>3662</v>
       </c>
       <c r="E11" s="8">
-        <v>4468</v>
+        <v>5946</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:E11" columnSort="0">
+    <sortCondition sortBy="value" descending="0" ref="A2:A11"/>
+  </sortState>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157500000008" bottom="0.78740157500000008" header="0.31496062000000014" footer="0.31496062000000014"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>

</xml_diff>

<commit_message>
adicionando tabelas de resultados
</commit_message>
<xml_diff>
--- a/resultados/resultados.xlsx
+++ b/resultados/resultados.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Berea200" sheetId="1" state="visible" r:id="rId1"/>
@@ -17,54 +17,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Imagem</t>
   </si>
   <si>
+    <t xml:space="preserve">Porosidade </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tempo Decorrido (s)</t>
+  </si>
+  <si>
+    <t>Poros</t>
+  </si>
+  <si>
+    <t>Solido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I22 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I212 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I26 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I216 </t>
+  </si>
+  <si>
     <t xml:space="preserve">Porosidade (%)</t>
   </si>
   <si>
-    <t xml:space="preserve">Tempo Decorrido (s)</t>
-  </si>
-  <si>
-    <t>Poros</t>
-  </si>
-  <si>
-    <t>Solido</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I22 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">I212 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">I26 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">I216 </t>
+    <t>I31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I310 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I311 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I312 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I318 </t>
   </si>
   <si>
     <t xml:space="preserve">I32 </t>
   </si>
   <si>
-    <t xml:space="preserve">I318 </t>
-  </si>
-  <si>
     <t xml:space="preserve">I320 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">I311 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">I312 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">I310 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">I31 </t>
   </si>
   <si>
     <t xml:space="preserve">3271i01 </t>
@@ -162,8 +165,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="160" formatCode="#,##0.000"/>
-    <numFmt numFmtId="161" formatCode="0.0000000"/>
+    <numFmt numFmtId="160" formatCode="0.000000"/>
+    <numFmt numFmtId="161" formatCode="#,##0.000"/>
     <numFmt numFmtId="162" formatCode="0.000"/>
   </numFmts>
   <fonts count="2">
@@ -201,14 +204,15 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="161" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="161" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="162" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
@@ -759,10 +763,10 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>0.30995768229166665</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
         <v>19.9934275150299</v>
       </c>
       <c r="D2">
@@ -776,10 +780,10 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>0.23840386025498497</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="3">
         <v>20.044158697128299</v>
       </c>
       <c r="D3">
@@ -793,10 +797,10 @@
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="4">
         <v>0.25565429687500002</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="3">
         <v>20.6440942287445</v>
       </c>
       <c r="D4">
@@ -810,10 +814,10 @@
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>0.25565429687500002</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="3">
         <v>20.760844707488999</v>
       </c>
       <c r="D5">
@@ -825,11 +829,11 @@
     </row>
     <row r="6" ht="14.25"/>
     <row r="7" ht="14.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" ht="14.25"/>
     <row r="9" ht="14.25"/>
@@ -853,7 +857,7 @@
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="21.140625"/>
-    <col customWidth="1" min="2" max="2" width="21.421875"/>
+    <col customWidth="1" min="2" max="2" width="15.28125"/>
     <col customWidth="1" min="3" max="3" width="22.7109375"/>
     <col customWidth="1" min="4" max="4" width="12.28125"/>
     <col customWidth="1" min="5" max="5" width="21.57421875"/>
@@ -863,143 +867,146 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="6">
-        <v>0.21280924479166666</v>
-      </c>
-      <c r="C2" s="7">
-        <v>19.897294998168945</v>
+      <c r="A2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.22181640624999999</v>
+      </c>
+      <c r="C2" s="8">
+        <v>20.364346504211426</v>
       </c>
       <c r="D2">
-        <v>4488</v>
+        <v>4025</v>
       </c>
       <c r="E2">
-        <v>5269</v>
+        <v>4457</v>
       </c>
     </row>
     <row r="3" ht="14.25">
       <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="6">
-        <v>0.24533203125</v>
-      </c>
-      <c r="C3" s="7">
-        <v>20.418896436691284</v>
+        <v>11</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.23427408854166668</v>
+      </c>
+      <c r="C3" s="8">
+        <v>20.360754489898682</v>
       </c>
       <c r="D3">
-        <v>3242</v>
+        <v>4367</v>
       </c>
       <c r="E3">
-        <v>4323</v>
+        <v>5604</v>
       </c>
     </row>
     <row r="4" ht="14.25">
       <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="6">
-        <v>0.144560546875</v>
-      </c>
-      <c r="C4" s="7">
-        <v>20.659868717193604</v>
+        <v>12</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.22600911458333334</v>
+      </c>
+      <c r="C4" s="8">
+        <v>20.79934549331665</v>
       </c>
       <c r="D4">
-        <v>3693</v>
+        <v>3138</v>
       </c>
       <c r="E4">
-        <v>4611</v>
+        <v>4710</v>
       </c>
     </row>
     <row r="5" ht="14.25">
       <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="6">
-        <v>0.22600911458333334</v>
-      </c>
-      <c r="C5" s="7">
-        <v>20.79934549331665</v>
+        <v>13</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.34716471354166667</v>
+      </c>
+      <c r="C5" s="8">
+        <v>20.709587097167969</v>
       </c>
       <c r="D5">
-        <v>3138</v>
+        <v>3848</v>
       </c>
       <c r="E5">
-        <v>4710</v>
+        <v>4199</v>
       </c>
     </row>
     <row r="6" ht="14.25">
       <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="6">
-        <v>0.34716471354166667</v>
-      </c>
-      <c r="C6" s="7">
-        <v>20.709587097167969</v>
+        <v>14</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.24533203125</v>
+      </c>
+      <c r="C6" s="8">
+        <v>20.418896436691284</v>
       </c>
       <c r="D6">
-        <v>3848</v>
+        <v>3242</v>
       </c>
       <c r="E6">
-        <v>4199</v>
+        <v>4323</v>
       </c>
     </row>
     <row r="7" ht="14.25">
       <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="6">
-        <v>0.23427408854166668</v>
-      </c>
-      <c r="C7" s="7">
-        <v>20.360754489898682</v>
+        <v>15</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.21280924479166666</v>
+      </c>
+      <c r="C7" s="8">
+        <v>19.897294998168945</v>
       </c>
       <c r="D7">
-        <v>4367</v>
+        <v>4488</v>
       </c>
       <c r="E7">
-        <v>5604</v>
+        <v>5269</v>
       </c>
     </row>
     <row r="8" ht="14.25">
       <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="6">
-        <v>0.22181640624999999</v>
-      </c>
-      <c r="C8" s="7">
-        <v>20.364346504211426</v>
+        <v>16</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.144560546875</v>
+      </c>
+      <c r="C8" s="8">
+        <v>20.659868717193604</v>
       </c>
       <c r="D8">
-        <v>4025</v>
+        <v>3693</v>
       </c>
       <c r="E8">
-        <v>4457</v>
+        <v>4611</v>
       </c>
     </row>
     <row r="9" ht="14.25"/>
   </sheetData>
+  <sortState ref="A2:E8" columnSort="0">
+    <sortCondition sortBy="value" descending="0" ref="A2:A8"/>
+  </sortState>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157500000008" bottom="0.78740157500000008" header="0.31496062000000014" footer="0.31496062000000014"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
@@ -1027,26 +1034,26 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" ht="14.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2">
         <v>0.24501953125000001</v>
@@ -1063,7 +1070,7 @@
     </row>
     <row r="3" ht="14.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3">
         <v>0.062360026041666669</v>
@@ -1080,7 +1087,7 @@
     </row>
     <row r="4" ht="14.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4">
         <v>0.20591471354166666</v>
@@ -1097,7 +1104,7 @@
     </row>
     <row r="5" ht="14.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5">
         <v>0.093710937499999994</v>
@@ -1114,7 +1121,7 @@
     </row>
     <row r="6" ht="14.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6">
         <v>0.24616536458333332</v>
@@ -1131,7 +1138,7 @@
     </row>
     <row r="7" ht="14.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7">
         <v>0.37842447916666666</v>
@@ -1148,7 +1155,7 @@
     </row>
     <row r="8" ht="14.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B8">
         <v>0.30426757812499999</v>
@@ -1165,7 +1172,7 @@
     </row>
     <row r="9" ht="14.25">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B9">
         <v>0.33873046875000001</v>
@@ -1182,7 +1189,7 @@
     </row>
     <row r="10" ht="14.25">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B10">
         <v>0.22583658854166666</v>
@@ -1199,7 +1206,7 @@
     </row>
     <row r="11" ht="14.25">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B11">
         <v>0.27026041666666667</v>
@@ -1244,189 +1251,189 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="8">
+      <c r="A2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="9">
         <v>0.27605794270833334</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="9">
         <v>19.107846975326538</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="9">
         <v>1906</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="9">
         <v>2257</v>
       </c>
     </row>
     <row r="3" ht="14.25">
-      <c r="A3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="8">
+      <c r="A3" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="9">
         <v>0.341064453125</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="9">
         <v>19.448724269866943</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="9">
         <v>1707</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="9">
         <v>2162</v>
       </c>
     </row>
     <row r="4" ht="14.25">
-      <c r="A4" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="8">
+      <c r="A4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="9">
         <v>0.27746744791666667</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="9">
         <v>19.24512243270874</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="9">
         <v>2651</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="9">
         <v>2898</v>
       </c>
     </row>
     <row r="5" ht="14.25">
-      <c r="A5" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="8">
+      <c r="A5" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="9">
         <v>0.31875976562500002</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="9">
         <v>19.038064241409302</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="9">
         <v>2220</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="9">
         <v>3189</v>
       </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="8">
+      <c r="A6" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="9">
         <v>0.25666666666666665</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="9">
         <v>19.21749210357666</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="9">
         <v>2033</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="9">
         <v>2168</v>
       </c>
     </row>
     <row r="7" ht="14.25">
-      <c r="A7" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="8">
+      <c r="A7" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="9">
         <v>0.28517578124999998</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="9">
         <v>19.658978462219238</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="9">
         <v>2516</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="9">
         <v>2517</v>
       </c>
     </row>
     <row r="8" ht="14.25">
-      <c r="A8" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="8">
+      <c r="A8" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="9">
         <v>0.43480468750000001</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="9">
         <v>19.249736785888672</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="9">
         <v>2691</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="9">
         <v>2311</v>
       </c>
     </row>
     <row r="9" ht="14.25">
-      <c r="A9" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="8">
+      <c r="A9" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="9">
         <v>0.35732421874999998</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="9">
         <v>19.931941032409668</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="9">
         <v>2294</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="9">
         <v>2275</v>
       </c>
     </row>
     <row r="10" ht="14.25">
-      <c r="A10" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="8">
+      <c r="A10" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="9">
         <v>0.27944010416666665</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="9">
         <v>19.275683641433716</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="9">
         <v>2673</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="9">
         <v>3429</v>
       </c>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="8">
+      <c r="A11" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="9">
         <v>0.33397135416666668</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="9">
         <v>19.238723993301392</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="9">
         <v>2112</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="9">
         <v>2426</v>
       </c>
     </row>
@@ -1460,189 +1467,189 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="8">
+      <c r="A2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="9">
         <v>0.20133789062499999</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="9">
         <v>21.443613290786743</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="9">
         <v>3022</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="9">
         <v>3948</v>
       </c>
     </row>
     <row r="3" ht="14.25">
-      <c r="A3" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="8">
+      <c r="A3" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="9">
         <v>0.19438476562500001</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="9">
         <v>21.069869041442871</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="9">
         <v>5921</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="9">
         <v>6761</v>
       </c>
     </row>
     <row r="4" ht="14.25">
-      <c r="A4" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="8">
+      <c r="A4" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="9">
         <v>0.16281901041666666</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="9">
         <v>21.49488353729248</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="9">
         <v>3024</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="9">
         <v>4209</v>
       </c>
     </row>
     <row r="5" ht="14.25">
-      <c r="A5" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="8">
+      <c r="A5" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="9">
         <v>0.16997721354166667</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="9">
         <v>20.347252130508423</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="9">
         <v>1900</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="9">
         <v>2963</v>
       </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6" s="8">
+      <c r="A6" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="9">
         <v>0.22072916666666667</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="9">
         <v>19.879645824432373</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="9">
         <v>3112</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="9">
         <v>4529</v>
       </c>
     </row>
     <row r="7" ht="14.25">
-      <c r="A7" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="8">
+      <c r="A7" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="9">
         <v>0.20756510416666665</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="9">
         <v>21.484671592712402</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="9">
         <v>2154</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="9">
         <v>3869</v>
       </c>
     </row>
     <row r="8" ht="14.25">
-      <c r="A8" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="8">
+      <c r="A8" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="9">
         <v>0.076256510416666673</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="9">
         <v>21.097349643707275</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="9">
         <v>1253</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="9">
         <v>4356</v>
       </c>
     </row>
     <row r="9" ht="14.25">
-      <c r="A9" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="8">
+      <c r="A9" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="9">
         <v>0.10691080729166667</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="9">
         <v>20.928617477416992</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="9">
         <v>3181</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="9">
         <v>5068</v>
       </c>
     </row>
     <row r="10" ht="14.25">
-      <c r="A10" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="8">
+      <c r="A10" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="9">
         <v>0.11185872395833334</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="9">
         <v>21.238481760025024</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="9">
         <v>2178</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="9">
         <v>4468</v>
       </c>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" s="8">
+      <c r="A11" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="9">
         <v>0.19612630208333334</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="9">
         <v>21.238434314727783</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="9">
         <v>3662</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="9">
         <v>5946</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adicionando análise dos resultados
</commit_message>
<xml_diff>
--- a/resultados/resultados.xlsx
+++ b/resultados/resultados.xlsx
@@ -12,12 +12,23 @@
     <sheet name="P240_K104" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="P262_K441" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="media4" hidden="0">P240_K104!$C$13</definedName>
+    <definedName name="esperada4" hidden="0">P240_K104!$EXP$4</definedName>
+    <definedName name="porosidade4" hidden="0">P240_K104!$C$16</definedName>
+    <definedName name="media3" hidden="0">P148_K2!$C$13</definedName>
+    <definedName name="porosidade3" hidden="0">P148_K2!$C$16</definedName>
+    <definedName name="media5" hidden="0">P262_K441!$C$13</definedName>
+    <definedName name="porosidade5" hidden="0">P262_K441!$C$16</definedName>
+    <definedName name="media1" hidden="0">Berea200!$C$7</definedName>
+    <definedName name="media2" hidden="0">Berea500!$C$10</definedName>
+  </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Imagem</t>
   </si>
@@ -25,6 +36,9 @@
     <t xml:space="preserve">Porosidade </t>
   </si>
   <si>
+    <t xml:space="preserve">Distancia da média</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tempo Decorrido (s)</t>
   </si>
   <si>
@@ -46,6 +60,12 @@
     <t xml:space="preserve">I216 </t>
   </si>
   <si>
+    <t>Média</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desvio Padrão</t>
+  </si>
+  <si>
     <t xml:space="preserve">Porosidade (%)</t>
   </si>
   <si>
@@ -70,6 +90,9 @@
     <t xml:space="preserve">I320 </t>
   </si>
   <si>
+    <t xml:space="preserve">Erro em relação ao valor real</t>
+  </si>
+  <si>
     <t xml:space="preserve">3271i01 </t>
   </si>
   <si>
@@ -98,6 +121,9 @@
   </si>
   <si>
     <t xml:space="preserve">3271i10 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Porosidade Esperada</t>
   </si>
   <si>
     <t xml:space="preserve">3251i01 </t>
@@ -164,10 +190,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="160" formatCode="0.000000"/>
-    <numFmt numFmtId="161" formatCode="#,##0.000"/>
-    <numFmt numFmtId="162" formatCode="0.000"/>
+    <numFmt numFmtId="161" formatCode="0.0000"/>
+    <numFmt numFmtId="162" formatCode="#,##0.000"/>
+    <numFmt numFmtId="163" formatCode="0.000"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -204,17 +231,34 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="161" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="161" xfId="0" applyNumberFormat="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="162" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="161" xfId="0" applyNumberFormat="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="162" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="163" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="163" xfId="0" applyNumberFormat="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
@@ -733,13 +777,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="9.7109375"/>
-    <col customWidth="1" min="2" max="2" width="15.00390625"/>
-    <col customWidth="1" min="3" max="3" width="19.00390625"/>
-    <col customWidth="1" min="4" max="4" width="9.140625"/>
-    <col customWidth="1" min="5" max="5" width="8.8515625"/>
-    <col customWidth="1" min="6" max="6" width="13.421875"/>
-    <col customWidth="1" min="7" max="7" width="12.28125"/>
+    <col customWidth="1" min="1" max="1" width="13.57421875"/>
+    <col customWidth="1" min="2" max="4" width="15.00390625"/>
+    <col customWidth="1" min="5" max="5" width="19.00390625"/>
+    <col customWidth="1" min="6" max="6" width="9.140625"/>
+    <col customWidth="1" min="7" max="7" width="8.8515625"/>
+    <col customWidth="1" min="8" max="8" width="13.421875"/>
+    <col customWidth="1" min="9" max="9" width="12.28125"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
@@ -749,96 +793,161 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="1"/>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" ht="14.25">
       <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="2">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3">
         <v>0.30995768229166665</v>
       </c>
       <c r="C2" s="3">
+        <f>100*B2</f>
+        <v>30.995768229166664</v>
+      </c>
+      <c r="D2" s="4">
+        <f>ABS(C2/media1*100-100)</f>
+        <v>17.001573102705564</v>
+      </c>
+      <c r="E2" s="5">
         <v>19.9934275150299</v>
       </c>
-      <c r="D2">
+      <c r="F2">
         <v>3059</v>
       </c>
-      <c r="E2">
+      <c r="G2">
         <v>4516</v>
       </c>
     </row>
     <row r="3" ht="14.25">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3">
         <v>0.23840386025498497</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="6">
+        <f>100*B3</f>
+        <v>23.840386025498496</v>
+      </c>
+      <c r="D3" s="7">
+        <f>ABS(C3/media1*100-100)</f>
+        <v>10.00827442843233</v>
+      </c>
+      <c r="E3" s="5">
         <v>20.044158697128299</v>
       </c>
-      <c r="D3">
+      <c r="F3">
         <v>4582</v>
       </c>
-      <c r="E3">
+      <c r="G3">
         <v>4556</v>
       </c>
     </row>
     <row r="4" ht="14.25">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="4">
+        <v>8</v>
+      </c>
+      <c r="B4" s="8">
         <v>0.25565429687500002</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="6">
+        <f>100*B4</f>
+        <v>25.565429687500004</v>
+      </c>
+      <c r="D4" s="7">
+        <f>ABS(C4/media1*100-100)</f>
+        <v>3.4966493371366028</v>
+      </c>
+      <c r="E4" s="5">
         <v>20.6440942287445</v>
       </c>
-      <c r="D4">
+      <c r="F4">
         <v>4059</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <v>4121</v>
       </c>
     </row>
     <row r="5" ht="14.25">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2">
+        <v>9</v>
+      </c>
+      <c r="B5" s="3">
         <v>0.25565429687500002</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="6">
+        <f>100*B5</f>
+        <v>25.565429687500004</v>
+      </c>
+      <c r="D5" s="7">
+        <f>ABS(C5/media1*100-100)</f>
+        <v>3.4966493371366028</v>
+      </c>
+      <c r="E5" s="5">
         <v>20.760844707488999</v>
       </c>
-      <c r="D5">
+      <c r="F5">
         <v>3695</v>
       </c>
-      <c r="E5">
+      <c r="G5">
         <v>4300</v>
       </c>
     </row>
-    <row r="6" ht="14.25"/>
+    <row r="6" ht="14.25">
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+    </row>
     <row r="7" ht="14.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" ht="14.25"/>
-    <row r="9" ht="14.25"/>
-    <row r="10" ht="14.25"/>
-    <row r="11" ht="14.25"/>
+      <c r="A7" s="10"/>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3">
+        <f>AVERAGE(C2:C5)</f>
+        <v>26.49175340741629</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="A8" s="11"/>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="12">
+        <f>STDEV(C2:C5)</f>
+        <v>3.1108439249719022</v>
+      </c>
+      <c r="D8" s="13"/>
+    </row>
+    <row r="9" ht="14.25">
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+    </row>
+    <row r="10" ht="14.25">
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+    </row>
+    <row r="11" ht="14.25">
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+    </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157500000008" bottom="0.78740157500000008" header="0.31496062000000014" footer="0.31496062000000014"/>
@@ -857,154 +966,235 @@
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="21.140625"/>
-    <col customWidth="1" min="2" max="2" width="15.28125"/>
-    <col customWidth="1" min="3" max="3" width="22.7109375"/>
-    <col customWidth="1" min="4" max="4" width="12.28125"/>
-    <col customWidth="1" min="5" max="5" width="21.57421875"/>
-    <col customWidth="1" min="6" max="6" width="14.7109375"/>
-    <col customWidth="1" min="7" max="7" width="13.421875"/>
-    <col customWidth="1" min="8" max="8" width="12.28125"/>
+    <col customWidth="1" min="2" max="4" width="15.28125"/>
+    <col customWidth="1" min="5" max="5" width="19.57421875"/>
+    <col customWidth="1" min="6" max="6" width="7.57421875"/>
+    <col customWidth="1" min="7" max="7" width="9.28125"/>
+    <col customWidth="1" min="8" max="8" width="14.7109375"/>
+    <col customWidth="1" min="9" max="9" width="13.421875"/>
+    <col customWidth="1" min="10" max="10" width="12.28125"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="2">
+      <c r="A2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="3">
         <v>0.22181640624999999</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="3">
+        <f>100*B2</f>
+        <v>22.181640625</v>
+      </c>
+      <c r="D2" s="4">
+        <f>ABS(C2/media2*100-100)</f>
+        <v>4.8561854230661794</v>
+      </c>
+      <c r="E2" s="14">
         <v>20.364346504211426</v>
       </c>
-      <c r="D2">
+      <c r="F2">
         <v>4025</v>
       </c>
-      <c r="E2">
+      <c r="G2">
         <v>4457</v>
       </c>
     </row>
     <row r="3" ht="14.25">
       <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="2">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3">
         <v>0.23427408854166668</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="3">
+        <f>100*B3</f>
+        <v>23.427408854166668</v>
+      </c>
+      <c r="D3" s="7">
+        <f>ABS(C3/media2*100-100)</f>
+        <v>0.48729405194080755</v>
+      </c>
+      <c r="E3" s="14">
         <v>20.360754489898682</v>
       </c>
-      <c r="D3">
+      <c r="F3">
         <v>4367</v>
       </c>
-      <c r="E3">
+      <c r="G3">
         <v>5604</v>
       </c>
     </row>
     <row r="4" ht="14.25">
       <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="2">
+        <v>15</v>
+      </c>
+      <c r="B4" s="3">
         <v>0.22600911458333334</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="3">
+        <f>100*B4</f>
+        <v>22.600911458333332</v>
+      </c>
+      <c r="D4" s="7">
+        <f>ABS(C4/media2*100-100)</f>
+        <v>3.0578050823792324</v>
+      </c>
+      <c r="E4" s="14">
         <v>20.79934549331665</v>
       </c>
-      <c r="D4">
+      <c r="F4">
         <v>3138</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <v>4710</v>
       </c>
     </row>
     <row r="5" ht="14.25">
       <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="2">
+        <v>16</v>
+      </c>
+      <c r="B5" s="3">
         <v>0.34716471354166667</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="3">
+        <f>100*B5</f>
+        <v>34.716471354166664</v>
+      </c>
+      <c r="D5" s="7">
+        <f>ABS(C5/media2*100-100)</f>
+        <v>48.909522479754258</v>
+      </c>
+      <c r="E5" s="14">
         <v>20.709587097167969</v>
       </c>
-      <c r="D5">
+      <c r="F5">
         <v>3848</v>
       </c>
-      <c r="E5">
+      <c r="G5">
         <v>4199</v>
       </c>
     </row>
     <row r="6" ht="14.25">
       <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="2">
+        <v>17</v>
+      </c>
+      <c r="B6" s="3">
         <v>0.24533203125</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="3">
+        <f>100*B6</f>
+        <v>24.533203125</v>
+      </c>
+      <c r="D6" s="7">
+        <f>ABS(C6/media2*100-100)</f>
+        <v>5.2303825746998029</v>
+      </c>
+      <c r="E6" s="14">
         <v>20.418896436691284</v>
       </c>
-      <c r="D6">
+      <c r="F6">
         <v>3242</v>
       </c>
-      <c r="E6">
+      <c r="G6">
         <v>4323</v>
       </c>
     </row>
     <row r="7" ht="14.25">
       <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="2">
+        <v>18</v>
+      </c>
+      <c r="B7" s="3">
         <v>0.21280924479166666</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="3">
+        <f>100*B7</f>
+        <v>21.280924479166664</v>
+      </c>
+      <c r="D7" s="7">
+        <f>ABS(C7/media2*100-100)</f>
+        <v>8.719631387880483</v>
+      </c>
+      <c r="E7" s="14">
         <v>19.897294998168945</v>
       </c>
-      <c r="D7">
+      <c r="F7">
         <v>4488</v>
       </c>
-      <c r="E7">
+      <c r="G7">
         <v>5269</v>
       </c>
     </row>
     <row r="8" ht="14.25">
       <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="2">
+        <v>19</v>
+      </c>
+      <c r="B8" s="3">
         <v>0.144560546875</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="3">
+        <f>100*B8</f>
+        <v>14.4560546875</v>
+      </c>
+      <c r="D8" s="7">
+        <f>ABS(C8/media2*100-100)</f>
+        <v>37.993577213068974</v>
+      </c>
+      <c r="E8" s="14">
         <v>20.659868717193604</v>
       </c>
-      <c r="D8">
+      <c r="F8">
         <v>3693</v>
       </c>
-      <c r="E8">
+      <c r="G8">
         <v>4611</v>
       </c>
     </row>
     <row r="9" ht="14.25"/>
+    <row r="10" ht="14.25">
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="3">
+        <f>AVERAGE(C2:C8)</f>
+        <v>23.313802083333332</v>
+      </c>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" ht="14.25">
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="12">
+        <f>STDEV(C2:C8)</f>
+        <v>5.9986525541389515</v>
+      </c>
+      <c r="D11" s="13"/>
+    </row>
+    <row r="12" ht="14.25"/>
   </sheetData>
-  <sortState ref="A2:E8" columnSort="0">
+  <sortState ref="A2:G8" columnSort="0">
     <sortCondition sortBy="value" descending="0" ref="A2:A8"/>
   </sortState>
   <printOptions headings="0" gridLines="0"/>
@@ -1024,205 +1214,366 @@
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="21.140625"/>
-    <col customWidth="1" min="2" max="2" width="18.00390625"/>
-    <col customWidth="1" min="3" max="3" width="19.8515625"/>
-    <col customWidth="1" min="4" max="4" width="12.28125"/>
-    <col customWidth="1" min="5" max="5" width="10.28125"/>
-    <col customWidth="1" min="6" max="6" width="14.7109375"/>
-    <col customWidth="1" min="7" max="7" width="13.421875"/>
-    <col customWidth="1" min="8" max="8" width="12.28125"/>
+    <col customWidth="1" min="2" max="5" width="14.421875"/>
+    <col customWidth="1" min="6" max="6" width="18.57421875"/>
+    <col customWidth="1" min="7" max="7" width="12.28125"/>
+    <col customWidth="1" min="8" max="8" width="10.28125"/>
+    <col customWidth="1" min="9" max="9" width="14.7109375"/>
+    <col customWidth="1" min="10" max="10" width="13.421875"/>
+    <col customWidth="1" min="11" max="11" width="12.28125"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9"/>
+      <c r="H1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="12"/>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2">
+      <c r="A2" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="3">
         <v>0.24501953125000001</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="3">
+        <f>100*B2</f>
+        <v>24.501953125</v>
+      </c>
+      <c r="D2" s="4">
+        <f>ABS(C2/media3*100-100)</f>
+        <v>3.3536736072587985</v>
+      </c>
+      <c r="E2" s="4">
+        <f>ABS(C2/porosidade3*100-100)</f>
+        <v>65.553737331081066</v>
+      </c>
+      <c r="F2" s="14">
         <v>20.62668776512146</v>
       </c>
-      <c r="D2">
+      <c r="G2">
         <v>1210</v>
       </c>
-      <c r="E2">
+      <c r="H2">
         <v>2382</v>
       </c>
     </row>
     <row r="3" ht="14.25">
       <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3">
+        <v>22</v>
+      </c>
+      <c r="B3" s="3">
         <v>0.062360026041666669</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
+        <f>100*B3</f>
+        <v>6.236002604166667</v>
+      </c>
+      <c r="D3" s="7">
+        <f>ABS(C3/media3*100-100)</f>
+        <v>73.695412178899204</v>
+      </c>
+      <c r="E3" s="7">
+        <f>ABS(C3/porosidade3*100-100)</f>
+        <v>57.864847269144143</v>
+      </c>
+      <c r="F3" s="14">
         <v>20.388940334320068</v>
       </c>
-      <c r="D3">
+      <c r="G3">
         <v>1918</v>
       </c>
-      <c r="E3">
+      <c r="H3">
         <v>2745</v>
       </c>
     </row>
     <row r="4" ht="14.25">
       <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4">
+        <v>23</v>
+      </c>
+      <c r="B4" s="3">
         <v>0.20591471354166666</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
+        <f>100*B4</f>
+        <v>20.591471354166664</v>
+      </c>
+      <c r="D4" s="7">
+        <f>ABS(C4/media3*100-100)</f>
+        <v>13.141446374726058</v>
+      </c>
+      <c r="E4" s="7">
+        <f>ABS(C4/porosidade3*100-100)</f>
+        <v>39.13156320382879</v>
+      </c>
+      <c r="F4" s="14">
         <v>20.686766862869263</v>
       </c>
-      <c r="D4">
+      <c r="G4">
         <v>1733</v>
       </c>
-      <c r="E4">
+      <c r="H4">
         <v>2557</v>
       </c>
     </row>
     <row r="5" ht="14.25">
       <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5">
+        <v>24</v>
+      </c>
+      <c r="B5" s="3">
         <v>0.093710937499999994</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
+        <f>100*B5</f>
+        <v>9.37109375</v>
+      </c>
+      <c r="D5" s="7">
+        <f>ABS(C5/media3*100-100)</f>
+        <v>60.471030213820029</v>
+      </c>
+      <c r="E5" s="7">
+        <f>ABS(C5/porosidade3*100-100)</f>
+        <v>36.681798986486491</v>
+      </c>
+      <c r="F5" s="14">
         <v>20.822933435440063</v>
       </c>
-      <c r="D5">
+      <c r="G5">
         <v>1342</v>
       </c>
-      <c r="E5">
+      <c r="H5">
         <v>2113</v>
       </c>
     </row>
     <row r="6" ht="14.25">
       <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6">
+        <v>25</v>
+      </c>
+      <c r="B6" s="3">
         <v>0.24616536458333332</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
+        <f>100*B6</f>
+        <v>24.616536458333332</v>
+      </c>
+      <c r="D6" s="7">
+        <f>ABS(C6/media3*100-100)</f>
+        <v>3.8370068490517468</v>
+      </c>
+      <c r="E6" s="7">
+        <f>ABS(C6/porosidade3*100-100)</f>
+        <v>66.327949042792767</v>
+      </c>
+      <c r="F6" s="14">
         <v>20.532556056976318</v>
       </c>
-      <c r="D6">
+      <c r="G6">
         <v>1541</v>
       </c>
-      <c r="E6">
+      <c r="H6">
         <v>2279</v>
       </c>
     </row>
     <row r="7" ht="14.25">
       <c r="A7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7">
+        <v>26</v>
+      </c>
+      <c r="B7" s="3">
         <v>0.37842447916666666</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="3">
+        <f>100*B7</f>
+        <v>37.842447916666664</v>
+      </c>
+      <c r="D7" s="7">
+        <f>ABS(C7/media3*100-100)</f>
+        <v>59.626295525322831</v>
+      </c>
+      <c r="E7" s="7">
+        <f>ABS(C7/porosidade3*100-100)</f>
+        <v>155.69221565315314</v>
+      </c>
+      <c r="F7" s="14">
         <v>20.930784940719604</v>
       </c>
-      <c r="D7">
+      <c r="G7">
         <v>1377</v>
       </c>
-      <c r="E7">
+      <c r="H7">
         <v>1765</v>
       </c>
     </row>
     <row r="8" ht="14.25">
       <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8">
+        <v>27</v>
+      </c>
+      <c r="B8" s="3">
         <v>0.30426757812499999</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="3">
+        <f>100*B8</f>
+        <v>30.4267578125</v>
+      </c>
+      <c r="D8" s="7">
+        <f>ABS(C8/media3*100-100)</f>
+        <v>28.34557228303558</v>
+      </c>
+      <c r="E8" s="7">
+        <f>ABS(C8/porosidade3*100-100)</f>
+        <v>105.58620143581078</v>
+      </c>
+      <c r="F8" s="14">
         <v>20.724771976470947</v>
       </c>
-      <c r="D8">
+      <c r="G8">
         <v>1386</v>
       </c>
-      <c r="E8">
+      <c r="H8">
         <v>2544</v>
       </c>
     </row>
     <row r="9" ht="14.25">
       <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9">
+        <v>28</v>
+      </c>
+      <c r="B9" s="3">
         <v>0.33873046875000001</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="3">
+        <f>100*B9</f>
+        <v>33.873046875</v>
+      </c>
+      <c r="D9" s="7">
+        <f>ABS(C9/media3*100-100)</f>
+        <v>42.882643393438798</v>
+      </c>
+      <c r="E9" s="7">
+        <f>ABS(C9/porosidade3*100-100)</f>
+        <v>128.87193834459461</v>
+      </c>
+      <c r="F9" s="14">
         <v>20.581314325332642</v>
       </c>
-      <c r="D9">
+      <c r="G9">
         <v>1484</v>
       </c>
-      <c r="E9">
+      <c r="H9">
         <v>1629</v>
       </c>
     </row>
     <row r="10" ht="14.25">
       <c r="A10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10">
+        <v>29</v>
+      </c>
+      <c r="B10" s="3">
         <v>0.22583658854166666</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
+        <f>100*B10</f>
+        <v>22.583658854166664</v>
+      </c>
+      <c r="D10" s="7">
+        <f>ABS(C10/media3*100-100)</f>
+        <v>4.7380388753714158</v>
+      </c>
+      <c r="E10" s="7">
+        <f>ABS(C10/porosidade3*100-100)</f>
+        <v>52.592289555180173</v>
+      </c>
+      <c r="F10" s="14">
         <v>19.478908061981201</v>
       </c>
-      <c r="D10">
+      <c r="G10">
         <v>1646</v>
       </c>
-      <c r="E10">
+      <c r="H10">
         <v>2137</v>
       </c>
     </row>
     <row r="11" ht="14.25">
       <c r="A11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11">
+        <v>30</v>
+      </c>
+      <c r="B11" s="3">
         <v>0.27026041666666667</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="3">
+        <f>100*B11</f>
+        <v>27.026041666666668</v>
+      </c>
+      <c r="D11" s="7">
+        <f>ABS(C11/media3*100-100)</f>
+        <v>14.000735984709124</v>
+      </c>
+      <c r="E11" s="7">
+        <f>ABS(C11/porosidade3*100-100)</f>
+        <v>82.608389639639626</v>
+      </c>
+      <c r="F11" s="14">
         <v>20.704411745071411</v>
       </c>
-      <c r="D11">
+      <c r="G11">
         <v>1179</v>
       </c>
-      <c r="E11">
+      <c r="H11">
         <v>2052</v>
       </c>
     </row>
+    <row r="13" ht="14.25">
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="3">
+        <f>AVERAGE(C2:C11)</f>
+        <v>23.706901041666661</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" ht="14.25">
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="12">
+        <f>STDEV(C2:C11)</f>
+        <v>9.9023687320100287</v>
+      </c>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+    </row>
+    <row r="16" ht="14.25">
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="12">
+        <v>14.800000000000001</v>
+      </c>
+      <c r="D16">
+        <f>ABS(C16/media3*100-100)</f>
+        <v>37.570920914598297</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:E11" columnSort="0">
+  <sortState ref="A2:H11" columnSort="0">
     <sortCondition sortBy="value" descending="0" ref="A2:A11"/>
   </sortState>
   <printOptions headings="0" gridLines="0"/>
@@ -1241,204 +1592,368 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="11.57421875"/>
-    <col customWidth="1" min="2" max="2" width="14.8515625"/>
-    <col customWidth="1" min="3" max="3" width="19.00390625"/>
-    <col customWidth="1" min="4" max="4" width="12.28125"/>
-    <col customWidth="1" min="5" max="5" width="10.7109375"/>
-    <col customWidth="1" min="6" max="6" width="13.421875"/>
+    <col customWidth="1" min="1" max="1" width="15.28125"/>
+    <col customWidth="1" min="2" max="2" width="19.7109375"/>
+    <col customWidth="1" min="3" max="3" width="10.140625"/>
+    <col customWidth="1" min="4" max="4" width="17.8515625"/>
+    <col customWidth="1" min="5" max="5" width="26.8515625"/>
+    <col customWidth="1" min="6" max="6" width="19.00390625"/>
     <col customWidth="1" min="7" max="7" width="12.28125"/>
+    <col customWidth="1" min="8" max="8" width="10.7109375"/>
+    <col customWidth="1" min="9" max="9" width="13.421875"/>
+    <col customWidth="1" min="10" max="10" width="12.28125"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="H1" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="9">
+      <c r="A2" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="12">
         <v>0.27605794270833334</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="4">
+        <f>100*B2</f>
+        <v>27.605794270833332</v>
+      </c>
+      <c r="D2" s="4">
+        <f>ABS(C2/media4*100-100)</f>
+        <v>12.660135101037412</v>
+      </c>
+      <c r="E2" s="4">
+        <f>ABS(C2/porosidade4*100-100)</f>
+        <v>15.024142795138886</v>
+      </c>
+      <c r="F2" s="15">
         <v>19.107846975326538</v>
       </c>
-      <c r="D2" s="9">
+      <c r="G2" s="12">
         <v>1906</v>
       </c>
-      <c r="E2" s="9">
+      <c r="H2" s="12">
         <v>2257</v>
       </c>
     </row>
     <row r="3" ht="14.25">
-      <c r="A3" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="9">
+      <c r="A3" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="12">
         <v>0.341064453125</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="7">
+        <f>100*B3</f>
+        <v>34.1064453125</v>
+      </c>
+      <c r="D3" s="7">
+        <f>ABS(C3/media4*100-100)</f>
+        <v>7.9067784303850601</v>
+      </c>
+      <c r="E3" s="7">
+        <f>ABS(C3/porosidade4*100-100)</f>
+        <v>42.110188802083314</v>
+      </c>
+      <c r="F3" s="15">
         <v>19.448724269866943</v>
       </c>
-      <c r="D3" s="9">
+      <c r="G3" s="12">
         <v>1707</v>
       </c>
-      <c r="E3" s="9">
+      <c r="H3" s="12">
         <v>2162</v>
       </c>
     </row>
     <row r="4" ht="14.25">
-      <c r="A4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="9">
+      <c r="A4" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="12">
         <v>0.27746744791666667</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="7">
+        <f>100*B4</f>
+        <v>27.746744791666668</v>
+      </c>
+      <c r="D4" s="7">
+        <f>ABS(C4/media4*100-100)</f>
+        <v>12.214192509194348</v>
+      </c>
+      <c r="E4" s="7">
+        <f>ABS(C4/porosidade4*100-100)</f>
+        <v>15.611436631944443</v>
+      </c>
+      <c r="F4" s="15">
         <v>19.24512243270874</v>
       </c>
-      <c r="D4" s="9">
+      <c r="G4" s="12">
         <v>2651</v>
       </c>
-      <c r="E4" s="9">
+      <c r="H4" s="12">
         <v>2898</v>
       </c>
     </row>
     <row r="5" ht="14.25">
-      <c r="A5" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="9">
+      <c r="A5" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="12">
         <v>0.31875976562500002</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="7">
+        <f>100*B5</f>
+        <v>31.875976562500004</v>
+      </c>
+      <c r="D5" s="7">
+        <f>ABS(C5/media4*100-100)</f>
+        <v>0.84996863983390369</v>
+      </c>
+      <c r="E5" s="7">
+        <f>ABS(C5/porosidade4*100-100)</f>
+        <v>32.816569010416686</v>
+      </c>
+      <c r="F5" s="15">
         <v>19.038064241409302</v>
       </c>
-      <c r="D5" s="9">
+      <c r="G5" s="12">
         <v>2220</v>
       </c>
-      <c r="E5" s="9">
+      <c r="H5" s="12">
         <v>3189</v>
       </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="12">
+        <v>0.25666666666666665</v>
+      </c>
+      <c r="C6" s="7">
+        <f>100*B6</f>
+        <v>25.666666666666664</v>
+      </c>
+      <c r="D6" s="7">
+        <f>ABS(C6/media4*100-100)</f>
+        <v>18.795192883044621</v>
+      </c>
+      <c r="E6" s="7">
+        <f>ABS(C6/porosidade4*100-100)</f>
+        <v>6.9444444444444429</v>
+      </c>
+      <c r="F6" s="16">
+        <v>19.21749210357666</v>
+      </c>
+      <c r="G6" s="12">
+        <v>2033</v>
+      </c>
+      <c r="H6" s="12">
+        <v>2168</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25">
+      <c r="A7" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="12">
+        <v>0.28517578124999998</v>
+      </c>
+      <c r="C7" s="7">
+        <f>100*B7</f>
+        <v>28.517578125</v>
+      </c>
+      <c r="D7" s="7">
+        <f>ABS(C7/media4*100-100)</f>
+        <v>9.7754117759740922</v>
+      </c>
+      <c r="E7" s="7">
+        <f>ABS(C7/porosidade4*100-100)</f>
+        <v>18.8232421875</v>
+      </c>
+      <c r="F7" s="15">
+        <v>19.658978462219238</v>
+      </c>
+      <c r="G7" s="12">
+        <v>2516</v>
+      </c>
+      <c r="H7" s="12">
+        <v>2517</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="A8" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="12">
+        <v>0.43480468750000001</v>
+      </c>
+      <c r="C8" s="7">
+        <f>100*B8</f>
+        <v>43.48046875</v>
+      </c>
+      <c r="D8" s="7">
+        <f>ABS(C8/media4*100-100)</f>
+        <v>37.564535514229476</v>
+      </c>
+      <c r="E8" s="7">
+        <f>ABS(C8/porosidade4*100-100)</f>
+        <v>81.168619791666686</v>
+      </c>
+      <c r="F8" s="15">
+        <v>19.249736785888672</v>
+      </c>
+      <c r="G8" s="12">
+        <v>2691</v>
+      </c>
+      <c r="H8" s="12">
+        <v>2311</v>
+      </c>
+    </row>
+    <row r="9" ht="14.25">
+      <c r="A9" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="12">
+        <v>0.35732421874999998</v>
+      </c>
+      <c r="C9" s="7">
+        <f>100*B9</f>
+        <v>35.732421875</v>
+      </c>
+      <c r="D9" s="7">
+        <f>ABS(C9/media4*100-100)</f>
+        <v>13.051081539521519</v>
+      </c>
+      <c r="E9" s="7">
+        <f>ABS(C9/porosidade4*100-100)</f>
+        <v>48.885091145833314</v>
+      </c>
+      <c r="F9" s="15">
+        <v>19.931941032409668</v>
+      </c>
+      <c r="G9" s="12">
+        <v>2294</v>
+      </c>
+      <c r="H9" s="12">
+        <v>2275</v>
+      </c>
+    </row>
+    <row r="10" ht="14.25">
+      <c r="A10" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="12">
+        <v>0.27944010416666665</v>
+      </c>
+      <c r="C10" s="7">
+        <f>100*B10</f>
+        <v>27.944010416666664</v>
+      </c>
+      <c r="D10" s="7">
+        <f>ABS(C10/media4*100-100)</f>
+        <v>11.590078858716552</v>
+      </c>
+      <c r="E10" s="7">
+        <f>ABS(C10/porosidade4*100-100)</f>
+        <v>16.4333767361111</v>
+      </c>
+      <c r="F10" s="15">
+        <v>19.275683641433716</v>
+      </c>
+      <c r="G10" s="12">
+        <v>2673</v>
+      </c>
+      <c r="H10" s="12">
+        <v>3429</v>
+      </c>
+    </row>
+    <row r="11" ht="14.25">
+      <c r="A11" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="12">
+        <v>0.33397135416666668</v>
+      </c>
+      <c r="C11" s="7">
+        <f>100*B11</f>
+        <v>33.397135416666671</v>
+      </c>
+      <c r="D11" s="7">
+        <f>ABS(C11/media4*100-100)</f>
+        <v>5.6626470039970087</v>
+      </c>
+      <c r="E11" s="7">
+        <f>ABS(C11/porosidade4*100-100)</f>
+        <v>39.1547309027778</v>
+      </c>
+      <c r="F11" s="15">
+        <v>19.238723993301392</v>
+      </c>
+      <c r="G11" s="12">
+        <v>2112</v>
+      </c>
+      <c r="H11" s="12">
+        <v>2426</v>
+      </c>
+    </row>
+    <row r="13" ht="14.25">
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="3">
+        <f>AVERAGE(C2:C11)</f>
+        <v>31.607324218750001</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" ht="14.25">
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="12">
+        <f>STDEV(C2:C11)</f>
+        <v>5.3404465346506891</v>
+      </c>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+    </row>
+    <row r="16" ht="14.25">
+      <c r="B16" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="9">
-        <v>0.25666666666666665</v>
-      </c>
-      <c r="C6" s="9">
-        <v>19.21749210357666</v>
-      </c>
-      <c r="D6" s="9">
-        <v>2033</v>
-      </c>
-      <c r="E6" s="9">
-        <v>2168</v>
-      </c>
-    </row>
-    <row r="7" ht="14.25">
-      <c r="A7" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="9">
-        <v>0.28517578124999998</v>
-      </c>
-      <c r="C7" s="9">
-        <v>19.658978462219238</v>
-      </c>
-      <c r="D7" s="9">
-        <v>2516</v>
-      </c>
-      <c r="E7" s="9">
-        <v>2517</v>
-      </c>
-    </row>
-    <row r="8" ht="14.25">
-      <c r="A8" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="9">
-        <v>0.43480468750000001</v>
-      </c>
-      <c r="C8" s="9">
-        <v>19.249736785888672</v>
-      </c>
-      <c r="D8" s="9">
-        <v>2691</v>
-      </c>
-      <c r="E8" s="9">
-        <v>2311</v>
-      </c>
-    </row>
-    <row r="9" ht="14.25">
-      <c r="A9" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="9">
-        <v>0.35732421874999998</v>
-      </c>
-      <c r="C9" s="9">
-        <v>19.931941032409668</v>
-      </c>
-      <c r="D9" s="9">
-        <v>2294</v>
-      </c>
-      <c r="E9" s="9">
-        <v>2275</v>
-      </c>
-    </row>
-    <row r="10" ht="14.25">
-      <c r="A10" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="9">
-        <v>0.27944010416666665</v>
-      </c>
-      <c r="C10" s="9">
-        <v>19.275683641433716</v>
-      </c>
-      <c r="D10" s="9">
-        <v>2673</v>
-      </c>
-      <c r="E10" s="9">
-        <v>3429</v>
-      </c>
-    </row>
-    <row r="11" ht="14.25">
-      <c r="A11" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="9">
-        <v>0.33397135416666668</v>
-      </c>
-      <c r="C11" s="9">
-        <v>19.238723993301392</v>
-      </c>
-      <c r="D11" s="9">
-        <v>2112</v>
-      </c>
-      <c r="E11" s="9">
-        <v>2426</v>
+      <c r="C16">
+        <v>24</v>
+      </c>
+      <c r="D16" s="4">
+        <f>ABS(C16/media4*100-100)</f>
+        <v>24.068232306223521</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:E11" columnSort="0">
+  <sortState ref="A2:H11" columnSort="0">
     <sortCondition sortBy="value" descending="0" ref="A2:A11"/>
   </sortState>
   <printOptions headings="0" gridLines="0"/>
@@ -1457,204 +1972,368 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="10.8515625"/>
-    <col customWidth="1" min="2" max="2" width="15.7109375"/>
-    <col customWidth="1" min="3" max="3" width="19.00390625"/>
-    <col customWidth="1" min="4" max="4" width="12.28125"/>
-    <col customWidth="1" min="5" max="5" width="10.140625"/>
-    <col customWidth="1" min="6" max="6" width="13.421875"/>
+    <col customWidth="1" min="1" max="1" width="13.8515625"/>
+    <col customWidth="1" min="2" max="5" width="15.7109375"/>
+    <col customWidth="1" min="6" max="6" width="19.00390625"/>
     <col customWidth="1" min="7" max="7" width="12.28125"/>
+    <col customWidth="1" min="8" max="8" width="10.140625"/>
+    <col customWidth="1" min="9" max="9" width="13.421875"/>
+    <col customWidth="1" min="10" max="10" width="12.28125"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="H1" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="9">
+      <c r="A2" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="12">
         <v>0.20133789062499999</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="4">
+        <f>100*B2</f>
+        <v>20.1337890625</v>
+      </c>
+      <c r="D2" s="4">
+        <f>ABS(C2/media5*100-100)</f>
+        <v>22.173608161894691</v>
+      </c>
+      <c r="E2" s="4">
+        <f>ABS(C2/porosidade5*100-100)</f>
+        <v>23.153476860687022</v>
+      </c>
+      <c r="F2" s="15">
         <v>21.443613290786743</v>
       </c>
-      <c r="D2" s="9">
+      <c r="G2" s="12">
         <v>3022</v>
       </c>
-      <c r="E2" s="9">
+      <c r="H2" s="12">
         <v>3948</v>
       </c>
     </row>
     <row r="3" ht="14.25">
-      <c r="A3" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="9">
+      <c r="A3" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="12">
         <v>0.19438476562500001</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="7">
+        <f>100*B3</f>
+        <v>19.4384765625</v>
+      </c>
+      <c r="D3" s="7">
+        <f>ABS(C3/media5*100-100)</f>
+        <v>17.95439057392025</v>
+      </c>
+      <c r="E3" s="7">
+        <f>ABS(C3/porosidade5*100-100)</f>
+        <v>25.807341364503813</v>
+      </c>
+      <c r="F3" s="15">
         <v>21.069869041442871</v>
       </c>
-      <c r="D3" s="9">
+      <c r="G3" s="12">
         <v>5921</v>
       </c>
-      <c r="E3" s="9">
+      <c r="H3" s="12">
         <v>6761</v>
       </c>
     </row>
     <row r="4" ht="14.25">
-      <c r="A4" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="9">
+      <c r="A4" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="12">
         <v>0.16281901041666666</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="7">
+        <f>100*B4</f>
+        <v>16.281901041666664</v>
+      </c>
+      <c r="D4" s="7">
+        <f>ABS(C4/media5*100-100)</f>
+        <v>1.1999881482652199</v>
+      </c>
+      <c r="E4" s="7">
+        <f>ABS(C4/porosidade5*100-100)</f>
+        <v>37.855339535623422</v>
+      </c>
+      <c r="F4" s="15">
         <v>21.49488353729248</v>
       </c>
-      <c r="D4" s="9">
+      <c r="G4" s="12">
         <v>3024</v>
       </c>
-      <c r="E4" s="9">
+      <c r="H4" s="12">
         <v>4209</v>
       </c>
     </row>
     <row r="5" ht="14.25">
-      <c r="A5" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="9">
+      <c r="A5" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="12">
         <v>0.16997721354166667</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="7">
+        <f>100*B5</f>
+        <v>16.997721354166668</v>
+      </c>
+      <c r="D5" s="7">
+        <f>ABS(C5/media5*100-100)</f>
+        <v>3.1436726550848846</v>
+      </c>
+      <c r="E5" s="7">
+        <f>ABS(C5/porosidade5*100-100)</f>
+        <v>35.123200938295156</v>
+      </c>
+      <c r="F5" s="15">
         <v>20.347252130508423</v>
       </c>
-      <c r="D5" s="9">
+      <c r="G5" s="12">
         <v>1900</v>
       </c>
-      <c r="E5" s="9">
+      <c r="H5" s="12">
         <v>2963</v>
       </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" s="9">
+      <c r="A6" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="12">
         <v>0.22072916666666667</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="7">
+        <f>100*B6</f>
+        <v>22.072916666666668</v>
+      </c>
+      <c r="D6" s="7">
+        <f>ABS(C6/media5*100-100)</f>
+        <v>33.940405526858996</v>
+      </c>
+      <c r="E6" s="7">
+        <f>ABS(C6/porosidade5*100-100)</f>
+        <v>15.752226463104321</v>
+      </c>
+      <c r="F6" s="15">
         <v>19.879645824432373</v>
       </c>
-      <c r="D6" s="9">
+      <c r="G6" s="12">
         <v>3112</v>
       </c>
-      <c r="E6" s="9">
+      <c r="H6" s="12">
         <v>4529</v>
       </c>
     </row>
     <row r="7" ht="14.25">
-      <c r="A7" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="9">
+      <c r="A7" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="12">
         <v>0.20756510416666665</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="7">
+        <f>100*B7</f>
+        <v>20.756510416666664</v>
+      </c>
+      <c r="D7" s="7">
+        <f>ABS(C7/media5*100-100)</f>
+        <v>25.952336273221974</v>
+      </c>
+      <c r="E7" s="7">
+        <f>ABS(C7/porosidade5*100-100)</f>
+        <v>20.776677798982192</v>
+      </c>
+      <c r="F7" s="15">
         <v>21.484671592712402</v>
       </c>
-      <c r="D7" s="9">
+      <c r="G7" s="12">
         <v>2154</v>
       </c>
-      <c r="E7" s="9">
+      <c r="H7" s="12">
         <v>3869</v>
       </c>
     </row>
     <row r="8" ht="14.25">
-      <c r="A8" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="9">
+      <c r="A8" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="12">
         <v>0.076256510416666673</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="7">
+        <f>100*B8</f>
+        <v>7.625651041666667</v>
+      </c>
+      <c r="D8" s="7">
+        <f>ABS(C8/media5*100-100)</f>
+        <v>53.726876771587442</v>
+      </c>
+      <c r="E8" s="7">
+        <f>ABS(C8/porosidade5*100-100)</f>
+        <v>70.89446167302799</v>
+      </c>
+      <c r="F8" s="15">
         <v>21.097349643707275</v>
       </c>
-      <c r="D8" s="9">
+      <c r="G8" s="12">
         <v>1253</v>
       </c>
-      <c r="E8" s="9">
+      <c r="H8" s="12">
         <v>4356</v>
       </c>
     </row>
     <row r="9" ht="14.25">
-      <c r="A9" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" s="9">
+      <c r="A9" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="12">
         <v>0.10691080729166667</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="7">
+        <f>100*B9</f>
+        <v>10.691080729166668</v>
+      </c>
+      <c r="D9" s="7">
+        <f>ABS(C9/media5*100-100)</f>
+        <v>35.125579006627092</v>
+      </c>
+      <c r="E9" s="7">
+        <f>ABS(C9/porosidade5*100-100)</f>
+        <v>59.194348361959278</v>
+      </c>
+      <c r="F9" s="15">
         <v>20.928617477416992</v>
       </c>
-      <c r="D9" s="9">
+      <c r="G9" s="12">
         <v>3181</v>
       </c>
-      <c r="E9" s="9">
+      <c r="H9" s="12">
         <v>5068</v>
       </c>
     </row>
     <row r="10" ht="14.25">
-      <c r="A10" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" s="9">
+      <c r="A10" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="12">
         <v>0.11185872395833334</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="7">
+        <f>100*B10</f>
+        <v>11.185872395833334</v>
+      </c>
+      <c r="D10" s="7">
+        <f>ABS(C10/media5*100-100)</f>
+        <v>32.123139524547909</v>
+      </c>
+      <c r="E10" s="7">
+        <f>ABS(C10/porosidade5*100-100)</f>
+        <v>57.305830550254448</v>
+      </c>
+      <c r="F10" s="15">
         <v>21.238481760025024</v>
       </c>
-      <c r="D10" s="9">
+      <c r="G10" s="12">
         <v>2178</v>
       </c>
-      <c r="E10" s="9">
+      <c r="H10" s="12">
         <v>4468</v>
       </c>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B11" s="9">
+      <c r="A11" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="12">
         <v>0.19612630208333334</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="7">
+        <f>100*B11</f>
+        <v>19.612630208333336</v>
+      </c>
+      <c r="D11" s="7">
+        <f>ABS(C11/media5*100-100)</f>
+        <v>19.011170260046811</v>
+      </c>
+      <c r="E11" s="7">
+        <f>ABS(C11/porosidade5*100-100)</f>
+        <v>25.142632792620859</v>
+      </c>
+      <c r="F11" s="15">
         <v>21.238434314727783</v>
       </c>
-      <c r="D11" s="9">
+      <c r="G11" s="12">
         <v>3662</v>
       </c>
-      <c r="E11" s="9">
+      <c r="H11" s="12">
         <v>5946</v>
       </c>
     </row>
+    <row r="13" ht="14.25">
+      <c r="A13"/>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="3">
+        <f>AVERAGE(C2:C11)</f>
+        <v>16.479654947916668</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" ht="14.25">
+      <c r="A14"/>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="12">
+        <f>STDEV(C2:C11)</f>
+        <v>4.9635508636796208</v>
+      </c>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+    </row>
+    <row r="16" ht="14.25">
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="12">
+        <v>26.199999999999999</v>
+      </c>
+      <c r="D16" s="4">
+        <f>ABS(C13/porosidade5*100-100)</f>
+        <v>37.100553633905839</v>
+      </c>
+      <c r="E16" s="13"/>
+    </row>
   </sheetData>
-  <sortState ref="A2:E11" columnSort="0">
+  <sortState ref="A2:H11" columnSort="0">
     <sortCondition sortBy="value" descending="0" ref="A2:A11"/>
   </sortState>
   <printOptions headings="0" gridLines="0"/>

</xml_diff>

<commit_message>
add results and conclusion to slide
</commit_message>
<xml_diff>
--- a/resultados/resultados.xlsx
+++ b/resultados/resultados.xlsx
@@ -240,8 +240,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="160" formatCode="0.000000%"/>
-    <numFmt numFmtId="161" formatCode="0.0000"/>
+    <numFmt numFmtId="160" formatCode="0.0000"/>
+    <numFmt numFmtId="161" formatCode="0.000000%"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -347,22 +347,20 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="2" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="29">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="1" applyNumberFormat="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="1" applyNumberFormat="1">
+    <xf fontId="0" fillId="2" borderId="0" numFmtId="10" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf fontId="0" fillId="2" borderId="0" numFmtId="10" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf fontId="0" fillId="2" borderId="0" numFmtId="10" xfId="1" applyNumberFormat="1" applyFill="1">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="161" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="161" xfId="0" applyNumberFormat="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
@@ -373,14 +371,11 @@
     </xf>
     <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="160" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="160" xfId="1" applyNumberFormat="1" applyBorder="1">
+    <xf fontId="0" fillId="2" borderId="1" numFmtId="10" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="2" borderId="1" numFmtId="10" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="160" xfId="1" applyNumberFormat="1" applyBorder="1">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -395,21 +390,23 @@
     <xf fontId="1" fillId="0" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="160" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf fontId="1" fillId="0" borderId="1" numFmtId="160" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="1" fillId="0" borderId="1" numFmtId="161" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="1" numFmtId="160" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf fontId="1" fillId="0" borderId="2" numFmtId="160" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="1" fillId="0" borderId="1" numFmtId="161" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="161" xfId="1" applyNumberFormat="1" applyBorder="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="1" fillId="0" borderId="2" numFmtId="161" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="3" numFmtId="160" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="1" fillId="0" borderId="3" numFmtId="161" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="4" numFmtId="160" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="1" fillId="0" borderId="4" numFmtId="161" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="5" numFmtId="160" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="1" fillId="0" borderId="5" numFmtId="161" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
@@ -988,21 +985,21 @@
       <c r="C3" s="4">
         <v>0.30995768229166665</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>0.36738281249999999</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>0.37379882812499998</v>
       </c>
       <c r="F3" s="4">
         <v>0.30995768229166665</v>
       </c>
-      <c r="G3" s="6">
-        <f>AVERAGE(B3:F3)</f>
+      <c r="G3" s="5">
+        <f t="shared" ref="G3:G6" si="0">AVERAGE(B3:F3)</f>
         <v>0.33421093750000008</v>
       </c>
-      <c r="H3" s="6">
-        <f>STDEV(B3:F3)</f>
+      <c r="H3" s="5">
+        <f t="shared" ref="H3:H6" si="1">STDEV(B3:F3)</f>
         <v>0.033287518455699786</v>
       </c>
     </row>
@@ -1016,21 +1013,21 @@
       <c r="C4" s="4">
         <v>0.23840386025498497</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>0.21516934233068302</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>0.33161563700627494</v>
       </c>
       <c r="F4" s="4">
         <v>0.23840386025498497</v>
       </c>
-      <c r="G4" s="6">
-        <f>AVERAGE(B4:F4)</f>
+      <c r="G4" s="5">
+        <f t="shared" si="0"/>
         <v>0.25239931202038257</v>
       </c>
-      <c r="H4" s="6">
-        <f>STDEV(B4:F4)</f>
+      <c r="H4" s="5">
+        <f t="shared" si="1"/>
         <v>0.045411768292258708</v>
       </c>
     </row>
@@ -1044,21 +1041,21 @@
       <c r="C5" s="4">
         <v>0.16578124999999999</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>0.22172851562500001</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>0.38314453124999998</v>
       </c>
       <c r="F5" s="4">
         <v>0.25565429687500002</v>
       </c>
-      <c r="G5" s="6">
-        <f>AVERAGE(B5:F5)</f>
+      <c r="G5" s="5">
+        <f t="shared" si="0"/>
         <v>0.23841796874999996</v>
       </c>
-      <c r="H5" s="6">
-        <f>STDEV(B5:F5)</f>
+      <c r="H5" s="5">
+        <f t="shared" si="1"/>
         <v>0.089545508775487781</v>
       </c>
     </row>
@@ -1072,79 +1069,79 @@
       <c r="C6" s="4">
         <v>0.25565429687500002</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>0.22639973958333334</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>0.26627278645833335</v>
       </c>
       <c r="F6" s="4">
         <v>0.25565429687500002</v>
       </c>
-      <c r="G6" s="6">
-        <f>AVERAGE(B6:F6)</f>
+      <c r="G6" s="5">
+        <f t="shared" si="0"/>
         <v>0.25192708333333336</v>
       </c>
-      <c r="H6" s="6">
-        <f>STDEV(B6:F6)</f>
+      <c r="H6" s="5">
+        <f t="shared" si="1"/>
         <v>0.014992671871925043</v>
       </c>
     </row>
     <row r="7" ht="14.25">
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="8"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
     </row>
     <row r="8" ht="14.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
     </row>
     <row r="9" ht="14.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
     </row>
     <row r="10" ht="14.25">
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="8"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
     </row>
     <row r="11" ht="14.25">
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="8"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
     </row>
     <row r="12" ht="14.25">
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="8"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
     </row>
     <row r="14" ht="14.25"/>
     <row r="15" ht="14.25"/>
@@ -1204,21 +1201,21 @@
       </c>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="7">
         <v>0.22181640624999999</v>
       </c>
-      <c r="C2" s="9">
-        <f t="shared" ref="C2:C8" si="0">100*B2</f>
+      <c r="C2" s="7">
+        <f t="shared" ref="C2:C8" si="2">100*B2</f>
         <v>22.181640625</v>
       </c>
-      <c r="D2" s="10">
-        <f t="shared" ref="D2:D8" si="1">ABS(C2/media2*100-100)</f>
+      <c r="D2" s="8">
+        <f t="shared" ref="D2:D8" si="3">ABS(C2/media2*100-100)</f>
         <v>4.8561854230661794</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="7">
         <v>9.7186565399169922</v>
       </c>
       <c r="F2">
@@ -1232,18 +1229,18 @@
       <c r="A3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="7">
         <v>0.23427408854166668</v>
       </c>
-      <c r="C3" s="9">
-        <f t="shared" si="0"/>
+      <c r="C3" s="7">
+        <f t="shared" si="2"/>
         <v>23.427408854166668</v>
       </c>
-      <c r="D3" s="10">
-        <f t="shared" si="1"/>
+      <c r="D3" s="8">
+        <f t="shared" si="3"/>
         <v>0.48729405194080755</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="7">
         <v>9.9234580993652344</v>
       </c>
       <c r="F3">
@@ -1257,18 +1254,18 @@
       <c r="A4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="7">
         <v>0.22600911458333334</v>
       </c>
-      <c r="C4" s="9">
-        <f t="shared" si="0"/>
+      <c r="C4" s="7">
+        <f t="shared" si="2"/>
         <v>22.600911458333332</v>
       </c>
-      <c r="D4" s="10">
-        <f t="shared" si="1"/>
+      <c r="D4" s="8">
+        <f t="shared" si="3"/>
         <v>3.0578050823792324</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="7">
         <v>9.9270343780517578</v>
       </c>
       <c r="F4">
@@ -1282,18 +1279,18 @@
       <c r="A5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="7">
         <v>0.34716471354166667</v>
       </c>
-      <c r="C5" s="9">
-        <f t="shared" si="0"/>
+      <c r="C5" s="7">
+        <f t="shared" si="2"/>
         <v>34.716471354166664</v>
       </c>
-      <c r="D5" s="10">
-        <f t="shared" si="1"/>
+      <c r="D5" s="8">
+        <f t="shared" si="3"/>
         <v>48.909522479754258</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="7">
         <v>9.3529224395751953</v>
       </c>
       <c r="F5">
@@ -1307,18 +1304,18 @@
       <c r="A6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="7">
         <v>0.24533203125</v>
       </c>
-      <c r="C6" s="9">
-        <f t="shared" si="0"/>
+      <c r="C6" s="7">
+        <f t="shared" si="2"/>
         <v>24.533203125</v>
       </c>
-      <c r="D6" s="10">
-        <f t="shared" si="1"/>
+      <c r="D6" s="8">
+        <f t="shared" si="3"/>
         <v>5.2303825746998029</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="7">
         <v>9.9303000000000008</v>
       </c>
       <c r="F6">
@@ -1332,18 +1329,18 @@
       <c r="A7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="7">
         <v>0.21280924479166666</v>
       </c>
-      <c r="C7" s="9">
-        <f t="shared" si="0"/>
+      <c r="C7" s="7">
+        <f t="shared" si="2"/>
         <v>21.280924479166664</v>
       </c>
-      <c r="D7" s="10">
-        <f t="shared" si="1"/>
+      <c r="D7" s="8">
+        <f t="shared" si="3"/>
         <v>8.719631387880483</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="7">
         <v>14.59074</v>
       </c>
       <c r="F7">
@@ -1357,18 +1354,18 @@
       <c r="A8" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="7">
         <v>0.144560546875</v>
       </c>
-      <c r="C8" s="9">
-        <f t="shared" si="0"/>
+      <c r="C8" s="7">
+        <f t="shared" si="2"/>
         <v>14.4560546875</v>
       </c>
-      <c r="D8" s="10">
-        <f t="shared" si="1"/>
+      <c r="D8" s="8">
+        <f t="shared" si="3"/>
         <v>37.993577213068974</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="7">
         <v>9.9575519561767578</v>
       </c>
       <c r="F8">
@@ -1383,12 +1380,12 @@
       <c r="B10" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="7">
         <f>AVERAGE(C2:C8)</f>
         <v>23.313802083333332</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9">
+      <c r="D10" s="7"/>
+      <c r="E10" s="7">
         <f>AVERAGE(E2:E8)</f>
         <v>10.485809059012277</v>
       </c>
@@ -1397,248 +1394,248 @@
       <c r="B11" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="8">
         <f>STDEV(C2:C8)</f>
         <v>5.9986525541389515</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="10">
+      <c r="D11" s="9"/>
+      <c r="E11" s="8">
         <f>STDEV(E2:E8)</f>
         <v>1.8229338412556984</v>
       </c>
     </row>
     <row r="12" ht="14.25"/>
     <row r="13" ht="14.25">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
     </row>
     <row r="14" ht="14.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="13" t="s">
+      <c r="A14" s="10"/>
+      <c r="B14" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="13" t="s">
+      <c r="F14" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="G14" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H14" s="13" t="s">
+      <c r="H14" s="11" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="15" ht="14.25">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="15">
+      <c r="B15" s="13">
         <v>0.22181640624999999</v>
       </c>
-      <c r="C15" s="15">
+      <c r="C15" s="13">
         <v>0.22181640624999999</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="13">
         <v>0.24033854166666666</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E15" s="13">
         <v>0.20912109374999999</v>
       </c>
-      <c r="F15" s="15">
+      <c r="F15" s="13">
         <v>0.22181640624999999</v>
       </c>
-      <c r="G15" s="16">
-        <f>AVERAGE(B15:F15)</f>
+      <c r="G15" s="14">
+        <f t="shared" ref="G15:G21" si="4">AVERAGE(B15:F15)</f>
         <v>0.22298177083333331</v>
       </c>
-      <c r="H15" s="16">
-        <f>STDEV(B15:F15)</f>
+      <c r="H15" s="14">
+        <f t="shared" ref="H15:H21" si="5">STDEV(B15:F15)</f>
         <v>0.011151794550716441</v>
       </c>
     </row>
     <row r="16" ht="14.25">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="15">
+      <c r="B16" s="13">
         <v>0.23427408854166668</v>
       </c>
-      <c r="C16" s="15">
+      <c r="C16" s="13">
         <v>0.23427408854166668</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="13">
         <v>0.35385742187500002</v>
       </c>
-      <c r="E16" s="15">
+      <c r="E16" s="13">
         <v>0.29802408854166668</v>
       </c>
-      <c r="F16" s="15">
+      <c r="F16" s="13">
         <v>0.23427408854166668</v>
       </c>
-      <c r="G16" s="18">
-        <f>AVERAGE(B16:F16)</f>
+      <c r="G16" s="14">
+        <f t="shared" si="4"/>
         <v>0.27094075520833338</v>
       </c>
-      <c r="H16" s="18">
-        <f>STDEV(B16:F16)</f>
+      <c r="H16" s="14">
+        <f t="shared" si="5"/>
         <v>0.053949082218534755</v>
       </c>
     </row>
     <row r="17" ht="14.25">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="15">
+      <c r="B17" s="13">
         <v>0.22600911458333334</v>
       </c>
-      <c r="C17" s="15">
+      <c r="C17" s="13">
         <v>0.22600911458333334</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="13">
         <v>0.301513671875</v>
       </c>
-      <c r="E17" s="15">
+      <c r="E17" s="13">
         <v>0.24058919270833334</v>
       </c>
-      <c r="F17" s="15">
+      <c r="F17" s="13">
         <v>0.22600911458333334</v>
       </c>
-      <c r="G17" s="18">
-        <f>AVERAGE(B17:F17)</f>
+      <c r="G17" s="14">
+        <f t="shared" si="4"/>
         <v>0.24402604166666669</v>
       </c>
-      <c r="H17" s="18">
-        <f>STDEV(B17:F17)</f>
+      <c r="H17" s="14">
+        <f t="shared" si="5"/>
         <v>0.032750834120335498</v>
       </c>
     </row>
     <row r="18" ht="14.25">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="15">
+      <c r="B18" s="13">
         <v>0.34716471354166667</v>
       </c>
-      <c r="C18" s="15">
+      <c r="C18" s="13">
         <v>0.34716471354166667</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="13">
         <v>0.39962565104166664</v>
       </c>
-      <c r="E18" s="15">
+      <c r="E18" s="13">
         <v>0.34086588541666668</v>
       </c>
-      <c r="F18" s="15">
+      <c r="F18" s="13">
         <v>0.34716471354166667</v>
       </c>
-      <c r="G18" s="18">
-        <f>AVERAGE(B18:F18)</f>
+      <c r="G18" s="14">
+        <f t="shared" si="4"/>
         <v>0.35639713541666668</v>
       </c>
-      <c r="H18" s="18">
-        <f>STDEV(B18:F18)</f>
+      <c r="H18" s="14">
+        <f t="shared" si="5"/>
         <v>0.024318907925404986</v>
       </c>
     </row>
     <row r="19" ht="14.25">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="15">
+      <c r="B19" s="13">
         <v>0.24533203125</v>
       </c>
-      <c r="C19" s="15">
+      <c r="C19" s="13">
         <v>0.24533203125</v>
       </c>
-      <c r="D19" s="15">
+      <c r="D19" s="13">
         <v>0.35010742187499999</v>
       </c>
-      <c r="E19" s="15">
+      <c r="E19" s="13">
         <v>0.28603190104166665</v>
       </c>
-      <c r="F19" s="15">
+      <c r="F19" s="13">
         <v>0.24533203125</v>
       </c>
-      <c r="G19" s="18">
-        <f>AVERAGE(B19:F19)</f>
+      <c r="G19" s="14">
+        <f t="shared" si="4"/>
         <v>0.27442708333333338</v>
       </c>
-      <c r="H19" s="18">
-        <f>STDEV(B19:F19)</f>
+      <c r="H19" s="14">
+        <f t="shared" si="5"/>
         <v>0.045830534589454006</v>
       </c>
     </row>
     <row r="20" ht="14.25">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="15">
+      <c r="B20" s="13">
         <v>0.21280924479166666</v>
       </c>
-      <c r="C20" s="15">
+      <c r="C20" s="13">
         <v>0.21280924479166666</v>
       </c>
-      <c r="D20" s="15">
+      <c r="D20" s="13">
         <v>0.26361002604166667</v>
       </c>
-      <c r="E20" s="15">
+      <c r="E20" s="13">
         <v>0.22496093750000001</v>
       </c>
-      <c r="F20" s="15">
+      <c r="F20" s="13">
         <v>0.21280924479166666</v>
       </c>
-      <c r="G20" s="18">
-        <f>AVERAGE(B20:F20)</f>
+      <c r="G20" s="14">
+        <f t="shared" si="4"/>
         <v>0.22539973958333331</v>
       </c>
-      <c r="H20" s="18">
-        <f>STDEV(B20:F20)</f>
+      <c r="H20" s="14">
+        <f t="shared" si="5"/>
         <v>0.021998751190653906</v>
       </c>
     </row>
     <row r="21" ht="14.25">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="15">
+      <c r="B21" s="13">
         <v>0.144560546875</v>
       </c>
-      <c r="C21" s="15">
+      <c r="C21" s="13">
         <v>0.144560546875</v>
       </c>
-      <c r="D21" s="15">
+      <c r="D21" s="13">
         <v>0.2632421875</v>
       </c>
-      <c r="E21" s="15">
+      <c r="E21" s="13">
         <v>0.22855794270833332</v>
       </c>
-      <c r="F21" s="15">
+      <c r="F21" s="13">
         <v>0.144560546875</v>
       </c>
-      <c r="G21" s="18">
-        <f>AVERAGE(B21:F21)</f>
+      <c r="G21" s="14">
+        <f t="shared" si="4"/>
         <v>0.18509635416666664</v>
       </c>
-      <c r="H21" s="18">
-        <f>STDEV(B21:F21)</f>
+      <c r="H21" s="14">
+        <f t="shared" si="5"/>
         <v>0.056844383988850757</v>
       </c>
     </row>
@@ -1704,28 +1701,28 @@
       <c r="H1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="11"/>
+      <c r="I1" s="9"/>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="7">
         <v>0.24501953125000001</v>
       </c>
-      <c r="C2" s="9">
-        <f t="shared" ref="C2:C9" si="2">100*B2</f>
+      <c r="C2" s="7">
+        <f t="shared" ref="C2:C9" si="6">100*B2</f>
         <v>24.501953125</v>
       </c>
-      <c r="D2" s="10">
-        <f t="shared" ref="D2:D9" si="3">ABS(C2/media3*100-100)</f>
+      <c r="D2" s="8">
+        <f t="shared" ref="D2:D9" si="7">ABS(C2/media3*100-100)</f>
         <v>3.3536736072587985</v>
       </c>
-      <c r="E2" s="10">
-        <f t="shared" ref="E2:E9" si="4">ABS(C2/porosidade3*100-100)</f>
+      <c r="E2" s="8">
+        <f t="shared" ref="E2:E9" si="8">ABS(C2/porosidade3*100-100)</f>
         <v>65.553737331081066</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="7">
         <v>10.281085968017578</v>
       </c>
       <c r="G2">
@@ -1739,22 +1736,22 @@
       <c r="A3" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="7">
         <v>0.062360026041666669</v>
       </c>
-      <c r="C3" s="9">
-        <f t="shared" si="2"/>
+      <c r="C3" s="7">
+        <f t="shared" si="6"/>
         <v>6.236002604166667</v>
       </c>
-      <c r="D3" s="10">
-        <f t="shared" si="3"/>
+      <c r="D3" s="8">
+        <f t="shared" si="7"/>
         <v>73.695412178899204</v>
       </c>
-      <c r="E3" s="10">
-        <f t="shared" si="4"/>
+      <c r="E3" s="8">
+        <f t="shared" si="8"/>
         <v>57.864847269144143</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="7">
         <v>10.356664657592773</v>
       </c>
       <c r="G3">
@@ -1768,22 +1765,22 @@
       <c r="A4" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="7">
         <v>0.20591471354166666</v>
       </c>
-      <c r="C4" s="9">
-        <f t="shared" si="2"/>
+      <c r="C4" s="7">
+        <f t="shared" si="6"/>
         <v>20.591471354166664</v>
       </c>
-      <c r="D4" s="10">
-        <f t="shared" si="3"/>
+      <c r="D4" s="8">
+        <f t="shared" si="7"/>
         <v>13.141446374726058</v>
       </c>
-      <c r="E4" s="10">
-        <f t="shared" si="4"/>
+      <c r="E4" s="8">
+        <f t="shared" si="8"/>
         <v>39.13156320382879</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="7">
         <v>10.334968566894531</v>
       </c>
       <c r="G4">
@@ -1797,22 +1794,22 @@
       <c r="A5" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="7">
         <v>0.093710937499999994</v>
       </c>
-      <c r="C5" s="9">
-        <f t="shared" si="2"/>
+      <c r="C5" s="7">
+        <f t="shared" si="6"/>
         <v>9.37109375</v>
       </c>
-      <c r="D5" s="10">
-        <f t="shared" si="3"/>
+      <c r="D5" s="8">
+        <f t="shared" si="7"/>
         <v>60.471030213820029</v>
       </c>
-      <c r="E5" s="10">
-        <f t="shared" si="4"/>
+      <c r="E5" s="8">
+        <f t="shared" si="8"/>
         <v>36.681798986486491</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="7">
         <v>10.259151458740234</v>
       </c>
       <c r="G5">
@@ -1826,22 +1823,22 @@
       <c r="A6" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="7">
         <v>0.24616536458333332</v>
       </c>
-      <c r="C6" s="9">
-        <f t="shared" si="2"/>
+      <c r="C6" s="7">
+        <f t="shared" si="6"/>
         <v>24.616536458333332</v>
       </c>
-      <c r="D6" s="10">
-        <f t="shared" si="3"/>
+      <c r="D6" s="8">
+        <f t="shared" si="7"/>
         <v>3.8370068490517468</v>
       </c>
-      <c r="E6" s="10">
-        <f t="shared" si="4"/>
+      <c r="E6" s="8">
+        <f t="shared" si="8"/>
         <v>66.327949042792767</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="7">
         <v>10.243892669677734</v>
       </c>
       <c r="G6">
@@ -1855,22 +1852,22 @@
       <c r="A7" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="7">
         <v>0.37842447916666666</v>
       </c>
-      <c r="C7" s="9">
-        <f t="shared" si="2"/>
+      <c r="C7" s="7">
+        <f t="shared" si="6"/>
         <v>37.842447916666664</v>
       </c>
-      <c r="D7" s="10">
-        <f t="shared" si="3"/>
+      <c r="D7" s="8">
+        <f t="shared" si="7"/>
         <v>59.626295525322831</v>
       </c>
-      <c r="E7" s="10">
-        <f t="shared" si="4"/>
+      <c r="E7" s="8">
+        <f t="shared" si="8"/>
         <v>155.69221565315314</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="7">
         <v>10.451316833496094</v>
       </c>
       <c r="G7">
@@ -1884,22 +1881,22 @@
       <c r="A8" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="7">
         <v>0.30426757812499999</v>
       </c>
-      <c r="C8" s="9">
-        <f t="shared" si="2"/>
+      <c r="C8" s="7">
+        <f t="shared" si="6"/>
         <v>30.4267578125</v>
       </c>
-      <c r="D8" s="10">
-        <f t="shared" si="3"/>
+      <c r="D8" s="8">
+        <f t="shared" si="7"/>
         <v>28.34557228303558</v>
       </c>
-      <c r="E8" s="10">
-        <f t="shared" si="4"/>
+      <c r="E8" s="8">
+        <f t="shared" si="8"/>
         <v>105.58620143581078</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="7">
         <v>10.221719741821289</v>
       </c>
       <c r="G8">
@@ -1913,22 +1910,22 @@
       <c r="A9" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="7">
         <v>0.33873046875000001</v>
       </c>
-      <c r="C9" s="9">
-        <f t="shared" si="2"/>
+      <c r="C9" s="7">
+        <f t="shared" si="6"/>
         <v>33.873046875</v>
       </c>
-      <c r="D9" s="10">
-        <f t="shared" si="3"/>
+      <c r="D9" s="8">
+        <f t="shared" si="7"/>
         <v>42.882643393438798</v>
       </c>
-      <c r="E9" s="10">
-        <f t="shared" si="4"/>
+      <c r="E9" s="8">
+        <f t="shared" si="8"/>
         <v>128.87193834459461</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="7">
         <v>10.05864143371582</v>
       </c>
       <c r="G9">
@@ -1942,22 +1939,22 @@
       <c r="A10" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="7">
         <v>0.22583658854166666</v>
       </c>
-      <c r="C10" s="9">
-        <f t="shared" ref="C10:C11" si="5">100*B10</f>
+      <c r="C10" s="7">
+        <f t="shared" ref="C10:C11" si="9">100*B10</f>
         <v>22.583658854166664</v>
       </c>
-      <c r="D10" s="10">
-        <f t="shared" ref="D10:D16" si="6">ABS(C10/media3*100-100)</f>
+      <c r="D10" s="8">
+        <f t="shared" ref="D10:D16" si="10">ABS(C10/media3*100-100)</f>
         <v>4.7380388753714158</v>
       </c>
-      <c r="E10" s="10">
-        <f t="shared" ref="E10:E11" si="7">ABS(C10/porosidade3*100-100)</f>
+      <c r="E10" s="8">
+        <f t="shared" ref="E10:E11" si="11">ABS(C10/porosidade3*100-100)</f>
         <v>52.592289555180173</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="7">
         <v>14.281272888183594</v>
       </c>
       <c r="G10">
@@ -1971,22 +1968,22 @@
       <c r="A11" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="7">
         <v>0.27026041666666667</v>
       </c>
-      <c r="C11" s="9">
-        <f t="shared" si="5"/>
+      <c r="C11" s="7">
+        <f t="shared" si="9"/>
         <v>27.026041666666668</v>
       </c>
-      <c r="D11" s="10">
-        <f t="shared" si="6"/>
+      <c r="D11" s="8">
+        <f t="shared" si="10"/>
         <v>14.000735984709124</v>
       </c>
-      <c r="E11" s="10">
-        <f t="shared" si="7"/>
+      <c r="E11" s="8">
+        <f t="shared" si="11"/>
         <v>82.608389639639626</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="7">
         <v>10.263204574584961</v>
       </c>
       <c r="G11">
@@ -2000,13 +1997,13 @@
       <c r="B13" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="7">
         <f>AVERAGE(C2:C11)</f>
         <v>23.706901041666661</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9">
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7">
         <f>AVERAGE(F2:F11)</f>
         <v>10.675191879272461</v>
       </c>
@@ -2015,13 +2012,13 @@
       <c r="B14" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="8">
         <f>STDEV(C2:C11)</f>
         <v>9.9023687320100287</v>
       </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="10">
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="8">
         <f>STDEV(F2:F11)</f>
         <v>1.2710924807586803</v>
       </c>
@@ -2030,329 +2027,329 @@
       <c r="B16" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="8">
         <v>14.800000000000001</v>
       </c>
-      <c r="D16" s="9">
-        <f t="shared" si="6"/>
+      <c r="D16" s="7">
+        <f t="shared" si="10"/>
         <v>37.570920914598297</v>
       </c>
     </row>
     <row r="18" ht="14.25">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="22"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="19"/>
     </row>
     <row r="19" ht="14.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="13" t="s">
+      <c r="A19" s="10"/>
+      <c r="B19" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F19" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H19" s="13" t="s">
+      <c r="H19" s="11" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="20" ht="14.25">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="15">
+      <c r="B20" s="13">
         <v>0.24501953125000001</v>
       </c>
-      <c r="C20" s="15">
+      <c r="C20" s="13">
         <v>0.24501953125000001</v>
       </c>
-      <c r="D20" s="15">
+      <c r="D20" s="13">
         <v>0.052747395833333335</v>
       </c>
-      <c r="E20" s="15">
+      <c r="E20" s="13">
         <v>0.27167954</v>
       </c>
       <c r="F20" s="3">
         <v>0.24501953125000001</v>
       </c>
-      <c r="G20" s="16">
-        <f>AVERAGE(B20:F20)</f>
+      <c r="G20" s="14">
+        <f t="shared" ref="G20:G29" si="12">AVERAGE(B20:F20)</f>
         <v>0.21189710591666669</v>
       </c>
-      <c r="H20" s="16">
-        <f>STDEV(B20:F20)</f>
+      <c r="H20" s="14">
+        <f t="shared" ref="H20:H29" si="13">STDEV(B20:F20)</f>
         <v>0.089713230384965897</v>
       </c>
     </row>
     <row r="21" ht="14.25">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="15">
+      <c r="B21" s="13">
         <v>0.062360026041666669</v>
       </c>
-      <c r="C21" s="15">
+      <c r="C21" s="13">
         <v>0.062360026041666669</v>
       </c>
-      <c r="D21" s="15">
+      <c r="D21" s="13">
         <v>0.12959960937500001</v>
       </c>
-      <c r="E21" s="15">
+      <c r="E21" s="13">
         <v>0.13484678999999999</v>
       </c>
       <c r="F21" s="3">
         <v>0.062360026041666669</v>
       </c>
-      <c r="G21" s="16">
-        <f>AVERAGE(B21:F21)</f>
+      <c r="G21" s="14">
+        <f t="shared" si="12"/>
         <v>0.090305295500000007</v>
       </c>
-      <c r="H21" s="16">
-        <f>STDEV(B21:F21)</f>
+      <c r="H21" s="14">
+        <f t="shared" si="13"/>
         <v>0.038310579774055629</v>
       </c>
     </row>
     <row r="22" ht="14.25">
-      <c r="A22" s="17" t="s">
+      <c r="A22" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="15">
+      <c r="B22" s="13">
         <v>0.20591471354166666</v>
       </c>
-      <c r="C22" s="15">
+      <c r="C22" s="13">
         <v>0.20591471354166666</v>
       </c>
-      <c r="D22" s="15">
+      <c r="D22" s="13">
         <v>0.16996419270833332</v>
       </c>
-      <c r="E22" s="15">
+      <c r="E22" s="13">
         <v>0.21426730999999999</v>
       </c>
       <c r="F22" s="3">
         <v>0.20591471354166666</v>
       </c>
-      <c r="G22" s="16">
-        <f>AVERAGE(B22:F22)</f>
+      <c r="G22" s="14">
+        <f t="shared" si="12"/>
         <v>0.20039512866666667</v>
       </c>
-      <c r="H22" s="16">
-        <f>STDEV(B22:F22)</f>
+      <c r="H22" s="14">
+        <f t="shared" si="13"/>
         <v>0.017391641166247456</v>
       </c>
     </row>
     <row r="23" ht="14.25">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="15">
+      <c r="B23" s="13">
         <v>0.093710937499999994</v>
       </c>
-      <c r="C23" s="15">
+      <c r="C23" s="13">
         <v>0.093710937499999994</v>
       </c>
-      <c r="D23" s="15">
+      <c r="D23" s="13">
         <v>0.11948242187499999</v>
       </c>
-      <c r="E23" s="15">
+      <c r="E23" s="13">
         <v>0.10154697600000001</v>
       </c>
       <c r="F23" s="3">
         <v>0.093710937499999994</v>
       </c>
-      <c r="G23" s="16">
-        <f>AVERAGE(B23:F23)</f>
+      <c r="G23" s="14">
+        <f t="shared" si="12"/>
         <v>0.10043244207499999</v>
       </c>
-      <c r="H23" s="16">
-        <f>STDEV(B23:F23)</f>
+      <c r="H23" s="14">
+        <f t="shared" si="13"/>
         <v>0.011176759229598061</v>
       </c>
     </row>
     <row r="24" ht="14.25">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="15">
+      <c r="B24" s="13">
         <v>0.24616536458333332</v>
       </c>
-      <c r="C24" s="15">
+      <c r="C24" s="13">
         <v>0.24616536458333332</v>
       </c>
-      <c r="D24" s="15">
+      <c r="D24" s="13">
         <v>0.29254882812499999</v>
       </c>
-      <c r="E24" s="15">
+      <c r="E24" s="13">
         <v>0.25564612341654563</v>
       </c>
       <c r="F24" s="3">
         <v>0.24616536458333332</v>
       </c>
-      <c r="G24" s="16">
-        <f>AVERAGE(B24:F24)</f>
+      <c r="G24" s="14">
+        <f t="shared" si="12"/>
         <v>0.25733820905830912</v>
       </c>
-      <c r="H24" s="16">
-        <f>STDEV(B24:F24)</f>
+      <c r="H24" s="14">
+        <f t="shared" si="13"/>
         <v>0.020106890671264095</v>
       </c>
     </row>
     <row r="25" ht="14.25">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="15">
+      <c r="B25" s="13">
         <v>0.37842447916666666</v>
       </c>
-      <c r="C25" s="15">
+      <c r="C25" s="13">
         <v>0.37842447916666666</v>
       </c>
-      <c r="D25" s="15">
+      <c r="D25" s="13">
         <v>0.32456963</v>
       </c>
-      <c r="E25" s="15">
+      <c r="E25" s="13">
         <v>0.31136547821646299</v>
       </c>
       <c r="F25" s="3">
         <v>0.37842447916666666</v>
       </c>
-      <c r="G25" s="16">
-        <f>AVERAGE(B25:F25)</f>
+      <c r="G25" s="14">
+        <f t="shared" si="12"/>
         <v>0.35424170914329262</v>
       </c>
-      <c r="H25" s="16">
-        <f>STDEV(B25:F25)</f>
+      <c r="H25" s="14">
+        <f t="shared" si="13"/>
         <v>0.033441077125246861</v>
       </c>
     </row>
     <row r="26" ht="14.25">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="15">
+      <c r="B26" s="13">
         <v>0.30426757812499999</v>
       </c>
-      <c r="C26" s="15">
+      <c r="C26" s="13">
         <v>0.30426757812499999</v>
       </c>
-      <c r="D26" s="15">
+      <c r="D26" s="13">
         <v>0.27480143229166665</v>
       </c>
-      <c r="E26" s="23">
+      <c r="E26" s="13">
         <v>0.37564117056455998</v>
       </c>
       <c r="F26" s="3">
         <v>0.30426757812499999</v>
       </c>
-      <c r="G26" s="16">
-        <f>AVERAGE(B26:F26)</f>
+      <c r="G26" s="14">
+        <f t="shared" si="12"/>
         <v>0.31264906744624532</v>
       </c>
-      <c r="H26" s="16">
-        <f>STDEV(B26:F26)</f>
+      <c r="H26" s="14">
+        <f t="shared" si="13"/>
         <v>0.037453960510835618</v>
       </c>
     </row>
     <row r="27" ht="14.25">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="15">
+      <c r="B27" s="13">
         <v>0.33873046875000001</v>
       </c>
-      <c r="C27" s="15">
+      <c r="C27" s="13">
         <v>0.33873046875000001</v>
       </c>
-      <c r="D27" s="15">
+      <c r="D27" s="13">
         <v>0.32205403645833336</v>
       </c>
-      <c r="E27" s="15">
+      <c r="E27" s="13">
         <v>0.31064032160653998</v>
       </c>
       <c r="F27" s="3">
         <v>0.33873046875000001</v>
       </c>
-      <c r="G27" s="18">
-        <f>AVERAGE(B27:F27)</f>
+      <c r="G27" s="14">
+        <f t="shared" si="12"/>
         <v>0.32977715286297471</v>
       </c>
-      <c r="H27" s="18">
-        <f>STDEV(B27:F27)</f>
+      <c r="H27" s="14">
+        <f t="shared" si="13"/>
         <v>0.012906882211203027</v>
       </c>
     </row>
     <row r="28" ht="14.25">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="15">
+      <c r="B28" s="13">
         <v>0.22583658854166666</v>
       </c>
-      <c r="C28" s="15">
+      <c r="C28" s="13">
         <v>0.22583658854166666</v>
       </c>
-      <c r="D28" s="15">
+      <c r="D28" s="13">
         <v>0.14849609375</v>
       </c>
-      <c r="E28" s="15">
+      <c r="E28" s="13">
         <v>0.22030316400399999</v>
       </c>
       <c r="F28" s="3">
         <v>0.22583658854166666</v>
       </c>
-      <c r="G28" s="18">
-        <f>AVERAGE(B28:F28)</f>
+      <c r="G28" s="14">
+        <f t="shared" si="12"/>
         <v>0.2092618046758</v>
       </c>
-      <c r="H28" s="18">
-        <f>STDEV(B28:F28)</f>
+      <c r="H28" s="14">
+        <f t="shared" si="13"/>
         <v>0.034053463923413498</v>
       </c>
     </row>
     <row r="29" ht="14.25">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="15">
+      <c r="B29" s="13">
         <v>0.27026041666666667</v>
       </c>
-      <c r="C29" s="15">
+      <c r="C29" s="13">
         <v>0.27026041666666667</v>
       </c>
-      <c r="D29" s="15">
+      <c r="D29" s="13">
         <v>0.2135709635416666</v>
       </c>
-      <c r="E29" s="15">
+      <c r="E29" s="13">
         <v>0.2506404478</v>
       </c>
       <c r="F29" s="3">
         <v>0.27026041666666667</v>
       </c>
-      <c r="G29" s="18">
-        <f>AVERAGE(B29:F29)</f>
+      <c r="G29" s="14">
+        <f t="shared" si="12"/>
         <v>0.25499853226833336</v>
       </c>
-      <c r="H29" s="18">
-        <f>STDEV(B29:F29)</f>
+      <c r="H29" s="14">
+        <f t="shared" si="13"/>
         <v>0.02466785203964917</v>
       </c>
     </row>
@@ -2417,295 +2414,295 @@
       <c r="H1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="11"/>
+      <c r="I1" s="9"/>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="8">
         <v>0.27605794270833334</v>
       </c>
-      <c r="C2" s="10">
-        <f t="shared" ref="C2:C9" si="8">100*B2</f>
+      <c r="C2" s="8">
+        <f t="shared" ref="C2:C9" si="14">100*B2</f>
         <v>27.605794270833332</v>
       </c>
-      <c r="D2" s="10">
-        <f t="shared" ref="D2:D9" si="9">ABS(C2/media4*100-100)</f>
+      <c r="D2" s="8">
+        <f t="shared" ref="D2:D9" si="15">ABS(C2/media4*100-100)</f>
         <v>12.660135101037412</v>
       </c>
-      <c r="E2" s="10">
-        <f t="shared" ref="E2:E9" si="10">ABS(C2/porosidade4*100-100)</f>
+      <c r="E2" s="8">
+        <f t="shared" ref="E2:E9" si="16">ABS(C2/porosidade4*100-100)</f>
         <v>15.024142795138886</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="8">
         <v>22.735118865966797</v>
       </c>
-      <c r="G2" s="11">
+      <c r="G2" s="9">
         <v>1906</v>
       </c>
-      <c r="H2" s="11">
+      <c r="H2" s="9">
         <v>2257</v>
       </c>
     </row>
     <row r="3" ht="14.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="8">
         <v>0.341064453125</v>
       </c>
-      <c r="C3" s="10">
-        <f t="shared" si="8"/>
+      <c r="C3" s="8">
+        <f t="shared" si="14"/>
         <v>34.1064453125</v>
       </c>
-      <c r="D3" s="10">
-        <f t="shared" si="9"/>
+      <c r="D3" s="8">
+        <f t="shared" si="15"/>
         <v>7.9067784303850601</v>
       </c>
-      <c r="E3" s="10">
-        <f t="shared" si="10"/>
+      <c r="E3" s="8">
+        <f t="shared" si="16"/>
         <v>42.110188802083314</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="8">
         <v>10.192632675170898</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="9">
         <v>1707</v>
       </c>
-      <c r="H3" s="11">
+      <c r="H3" s="9">
         <v>2162</v>
       </c>
     </row>
     <row r="4" ht="14.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="8">
         <v>0.27746744791666667</v>
       </c>
-      <c r="C4" s="10">
-        <f t="shared" si="8"/>
+      <c r="C4" s="8">
+        <f t="shared" si="14"/>
         <v>27.746744791666668</v>
       </c>
-      <c r="D4" s="10">
-        <f t="shared" si="9"/>
+      <c r="D4" s="8">
+        <f t="shared" si="15"/>
         <v>12.214192509194348</v>
       </c>
-      <c r="E4" s="10">
-        <f t="shared" si="10"/>
+      <c r="E4" s="8">
+        <f t="shared" si="16"/>
         <v>15.611436631944443</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="8">
         <v>10.44917106628418</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="9">
         <v>2651</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="9">
         <v>2898</v>
       </c>
     </row>
     <row r="5" ht="14.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="8">
         <v>0.31875976562500002</v>
       </c>
-      <c r="C5" s="10">
-        <f t="shared" si="8"/>
+      <c r="C5" s="8">
+        <f t="shared" si="14"/>
         <v>31.875976562500004</v>
       </c>
-      <c r="D5" s="10">
-        <f t="shared" si="9"/>
+      <c r="D5" s="8">
+        <f t="shared" si="15"/>
         <v>0.84996863983390369</v>
       </c>
-      <c r="E5" s="10">
-        <f t="shared" si="10"/>
+      <c r="E5" s="8">
+        <f t="shared" si="16"/>
         <v>32.816569010416686</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="8">
         <v>10.275840759277344</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="9">
         <v>2220</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="9">
         <v>3189</v>
       </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="8">
         <v>0.25666666666666665</v>
       </c>
-      <c r="C6" s="10">
-        <f t="shared" si="8"/>
+      <c r="C6" s="8">
+        <f t="shared" si="14"/>
         <v>25.666666666666664</v>
       </c>
-      <c r="D6" s="10">
-        <f t="shared" si="9"/>
+      <c r="D6" s="8">
+        <f t="shared" si="15"/>
         <v>18.795192883044621</v>
       </c>
-      <c r="E6" s="10">
-        <f t="shared" si="10"/>
+      <c r="E6" s="8">
+        <f t="shared" si="16"/>
         <v>6.9444444444444429</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="8">
         <v>10.242938995361328</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="9">
         <v>2033</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="9">
         <v>2168</v>
       </c>
     </row>
     <row r="7" ht="14.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="8">
         <v>0.28517578124999998</v>
       </c>
-      <c r="C7" s="10">
-        <f t="shared" si="8"/>
+      <c r="C7" s="8">
+        <f t="shared" si="14"/>
         <v>28.517578125</v>
       </c>
-      <c r="D7" s="10">
-        <f t="shared" si="9"/>
+      <c r="D7" s="8">
+        <f t="shared" si="15"/>
         <v>9.7754117759740922</v>
       </c>
-      <c r="E7" s="10">
-        <f t="shared" si="10"/>
+      <c r="E7" s="8">
+        <f t="shared" si="16"/>
         <v>18.8232421875</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="8">
         <v>10.405302047729492</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="9">
         <v>2516</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="9">
         <v>2517</v>
       </c>
     </row>
     <row r="8" ht="14.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="8">
         <v>0.43480468750000001</v>
       </c>
-      <c r="C8" s="10">
-        <f t="shared" si="8"/>
+      <c r="C8" s="8">
+        <f t="shared" si="14"/>
         <v>43.48046875</v>
       </c>
-      <c r="D8" s="10">
-        <f t="shared" si="9"/>
+      <c r="D8" s="8">
+        <f t="shared" si="15"/>
         <v>37.564535514229476</v>
       </c>
-      <c r="E8" s="10">
-        <f t="shared" si="10"/>
+      <c r="E8" s="8">
+        <f t="shared" si="16"/>
         <v>81.168619791666686</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="8">
         <v>10.652780532836914</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="9">
         <v>2691</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="9">
         <v>2311</v>
       </c>
     </row>
     <row r="9" ht="14.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="8">
         <v>0.35732421874999998</v>
       </c>
-      <c r="C9" s="10">
-        <f t="shared" si="8"/>
+      <c r="C9" s="8">
+        <f t="shared" si="14"/>
         <v>35.732421875</v>
       </c>
-      <c r="D9" s="10">
-        <f t="shared" si="9"/>
+      <c r="D9" s="8">
+        <f t="shared" si="15"/>
         <v>13.051081539521519</v>
       </c>
-      <c r="E9" s="10">
-        <f t="shared" si="10"/>
+      <c r="E9" s="8">
+        <f t="shared" si="16"/>
         <v>48.885091145833314</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="8">
         <v>14.628410339355469</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="9">
         <v>2294</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="9">
         <v>2275</v>
       </c>
     </row>
     <row r="10" ht="14.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="8">
         <v>0.27944010416666665</v>
       </c>
-      <c r="C10" s="10">
-        <f t="shared" ref="C10:C11" si="11">100*B10</f>
+      <c r="C10" s="8">
+        <f t="shared" ref="C10:C11" si="17">100*B10</f>
         <v>27.944010416666664</v>
       </c>
-      <c r="D10" s="10">
-        <f t="shared" ref="D10:D16" si="12">ABS(C10/media4*100-100)</f>
+      <c r="D10" s="8">
+        <f t="shared" ref="D10:D16" si="18">ABS(C10/media4*100-100)</f>
         <v>11.590078858716552</v>
       </c>
-      <c r="E10" s="10">
-        <f t="shared" ref="E10:E11" si="13">ABS(C10/porosidade4*100-100)</f>
+      <c r="E10" s="8">
+        <f t="shared" ref="E10:E11" si="19">ABS(C10/porosidade4*100-100)</f>
         <v>16.4333767361111</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="8">
         <v>10.166168212890625</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="9">
         <v>2673</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="9">
         <v>3429</v>
       </c>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="8">
         <v>0.33397135416666668</v>
       </c>
-      <c r="C11" s="10">
-        <f t="shared" si="11"/>
+      <c r="C11" s="8">
+        <f t="shared" si="17"/>
         <v>33.397135416666671</v>
       </c>
-      <c r="D11" s="10">
-        <f t="shared" si="12"/>
+      <c r="D11" s="8">
+        <f t="shared" si="18"/>
         <v>5.6626470039970087</v>
       </c>
-      <c r="E11" s="10">
-        <f t="shared" si="13"/>
+      <c r="E11" s="8">
+        <f t="shared" si="19"/>
         <v>39.1547309027778</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="8">
         <v>10.244607925415039</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="9">
         <v>2112</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="9">
         <v>2426</v>
       </c>
     </row>
@@ -2713,13 +2710,13 @@
       <c r="B13" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="7">
         <f>AVERAGE(C2:C11)</f>
         <v>31.607324218750001</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9">
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7">
         <f>AVERAGE(F2:F11)</f>
         <v>11.999297142028809</v>
       </c>
@@ -2728,13 +2725,13 @@
       <c r="B14" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="8">
         <f>STDEV(C2:C11)</f>
         <v>5.3404465346506891</v>
       </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="10">
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="8">
         <f>STDEV(F2:F11)</f>
         <v>4.0095074612847448</v>
       </c>
@@ -2743,329 +2740,329 @@
       <c r="B16" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="7">
         <v>24</v>
       </c>
-      <c r="D16" s="10">
-        <f t="shared" si="12"/>
+      <c r="D16" s="8">
+        <f t="shared" si="18"/>
         <v>24.068232306223521</v>
       </c>
     </row>
     <row r="19" ht="14.25">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
     </row>
     <row r="20" ht="14.25">
-      <c r="A20" s="24"/>
-      <c r="B20" s="25" t="s">
+      <c r="A20" s="20"/>
+      <c r="B20" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="25" t="s">
+      <c r="C20" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="25" t="s">
+      <c r="D20" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="25" t="s">
+      <c r="E20" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="25" t="s">
+      <c r="F20" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="G20" s="25" t="s">
+      <c r="G20" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="21" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="21" ht="14.25">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="15">
+      <c r="B21" s="13">
         <v>0.27605794270833334</v>
       </c>
-      <c r="C21" s="15">
+      <c r="C21" s="13">
         <v>0.27605794270833334</v>
       </c>
-      <c r="D21" s="15">
+      <c r="D21" s="13">
         <v>0.37302408854166669</v>
       </c>
-      <c r="E21" s="15">
+      <c r="E21" s="13">
         <v>0.34314778645833333</v>
       </c>
-      <c r="F21" s="15">
+      <c r="F21" s="13">
         <v>0.34738281250000003</v>
       </c>
-      <c r="G21" s="16">
-        <f>AVERAGE(B21:F21)</f>
+      <c r="G21" s="14">
+        <f t="shared" ref="G21:G30" si="20">AVERAGE(B21:F21)</f>
         <v>0.32313411458333335</v>
       </c>
-      <c r="H21" s="16">
-        <f>STDEV(B21:F21)</f>
+      <c r="H21" s="14">
+        <f t="shared" ref="H21:H30" si="21">STDEV(B21:F21)</f>
         <v>0.044468775086981494</v>
       </c>
     </row>
     <row r="22" ht="14.25">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="15">
+      <c r="B22" s="13">
         <v>0.341064453125</v>
       </c>
-      <c r="C22" s="15">
+      <c r="C22" s="13">
         <v>0.341064453125</v>
       </c>
-      <c r="D22" s="15">
+      <c r="D22" s="13">
         <v>0.38645507812500002</v>
       </c>
-      <c r="E22" s="15">
+      <c r="E22" s="13">
         <v>0.36403645833333331</v>
       </c>
-      <c r="F22" s="15">
+      <c r="F22" s="13">
         <v>0.359130859375</v>
       </c>
-      <c r="G22" s="16">
-        <f>AVERAGE(B22:F22)</f>
+      <c r="G22" s="14">
+        <f t="shared" si="20"/>
         <v>0.35835026041666668</v>
       </c>
-      <c r="H22" s="16">
-        <f>STDEV(B22:F22)</f>
+      <c r="H22" s="14">
+        <f t="shared" si="21"/>
         <v>0.018844238027505757</v>
       </c>
     </row>
     <row r="23" ht="14.25">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="15">
+      <c r="B23" s="13">
         <v>0.27746744791666667</v>
       </c>
-      <c r="C23" s="15">
+      <c r="C23" s="13">
         <v>0.27746744791666667</v>
       </c>
-      <c r="D23" s="15">
+      <c r="D23" s="13">
         <v>0.34474283854166665</v>
       </c>
-      <c r="E23" s="15">
+      <c r="E23" s="13">
         <v>0.33485677083333332</v>
       </c>
-      <c r="F23" s="15">
+      <c r="F23" s="13">
         <v>0.32782877604166666</v>
       </c>
-      <c r="G23" s="16">
-        <f>AVERAGE(B23:F23)</f>
+      <c r="G23" s="14">
+        <f t="shared" si="20"/>
         <v>0.31247265625000004</v>
       </c>
-      <c r="H23" s="16">
-        <f>STDEV(B23:F23)</f>
+      <c r="H23" s="14">
+        <f t="shared" si="21"/>
         <v>0.032515199856349285</v>
       </c>
     </row>
     <row r="24" ht="14.25">
-      <c r="A24" s="16" t="s">
+      <c r="A24" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="15">
+      <c r="B24" s="13">
         <v>0.31875976562500002</v>
       </c>
-      <c r="C24" s="15">
+      <c r="C24" s="13">
         <v>0.31875976562500002</v>
       </c>
-      <c r="D24" s="15">
+      <c r="D24" s="13">
         <v>0.34299804687500002</v>
       </c>
-      <c r="E24" s="15">
+      <c r="E24" s="13">
         <v>0.34474283854166665</v>
       </c>
-      <c r="F24" s="15">
+      <c r="F24" s="13">
         <v>0.34596679687499998</v>
       </c>
-      <c r="G24" s="16">
-        <f>AVERAGE(B24:F24)</f>
+      <c r="G24" s="14">
+        <f t="shared" si="20"/>
         <v>0.33424544270833334</v>
       </c>
-      <c r="H24" s="16">
-        <f>STDEV(B24:F24)</f>
+      <c r="H24" s="14">
+        <f t="shared" si="21"/>
         <v>0.014175735712292125</v>
       </c>
     </row>
     <row r="25" ht="14.25">
-      <c r="A25" s="16" t="s">
+      <c r="A25" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="15">
+      <c r="B25" s="13">
         <v>0.25666666666666665</v>
       </c>
-      <c r="C25" s="15">
+      <c r="C25" s="13">
         <v>0.25666666666666665</v>
       </c>
-      <c r="D25" s="15">
+      <c r="D25" s="13">
         <v>0.31145182291666668</v>
       </c>
-      <c r="E25" s="15">
+      <c r="E25" s="13">
         <v>0.30605143229166665</v>
       </c>
-      <c r="F25" s="15">
+      <c r="F25" s="13">
         <v>0.30664388020833333</v>
       </c>
-      <c r="G25" s="16">
-        <f>AVERAGE(B25:F25)</f>
+      <c r="G25" s="14">
+        <f t="shared" si="20"/>
         <v>0.28749609374999996</v>
       </c>
-      <c r="H25" s="16">
-        <f>STDEV(B25:F25)</f>
+      <c r="H25" s="14">
+        <f t="shared" si="21"/>
         <v>0.028221102136210117</v>
       </c>
     </row>
     <row r="26" ht="14.25">
-      <c r="A26" s="16" t="s">
+      <c r="A26" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="15">
+      <c r="B26" s="13">
         <v>0.28517578124999998</v>
       </c>
-      <c r="C26" s="15">
+      <c r="C26" s="13">
         <v>0.28517578124999998</v>
       </c>
-      <c r="D26" s="15">
+      <c r="D26" s="13">
         <v>0.35605794270833335</v>
       </c>
-      <c r="E26" s="15">
+      <c r="E26" s="13">
         <v>0.34731119791666665</v>
       </c>
-      <c r="F26" s="15">
+      <c r="F26" s="13">
         <v>0.34659830729166669</v>
       </c>
-      <c r="G26" s="16">
-        <f>AVERAGE(B26:F26)</f>
+      <c r="G26" s="14">
+        <f t="shared" si="20"/>
         <v>0.32406380208333335</v>
       </c>
-      <c r="H26" s="16">
-        <f>STDEV(B26:F26)</f>
+      <c r="H26" s="14">
+        <f t="shared" si="21"/>
         <v>0.035694630902335649</v>
       </c>
     </row>
     <row r="27" ht="14.25">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="15">
+      <c r="B27" s="13">
         <v>0.43480468750000001</v>
       </c>
-      <c r="C27" s="15">
+      <c r="C27" s="13">
         <v>0.43480468750000001</v>
       </c>
-      <c r="D27" s="15">
+      <c r="D27" s="13">
         <v>0.38201822916666667</v>
       </c>
-      <c r="E27" s="15">
+      <c r="E27" s="13">
         <v>0.36209309895833336</v>
       </c>
-      <c r="F27" s="15">
+      <c r="F27" s="13">
         <v>0.35993164062499999</v>
       </c>
-      <c r="G27" s="16">
-        <f>AVERAGE(B27:F27)</f>
+      <c r="G27" s="14">
+        <f t="shared" si="20"/>
         <v>0.39473046875000001</v>
       </c>
-      <c r="H27" s="16">
-        <f>STDEV(B27:F27)</f>
+      <c r="H27" s="14">
+        <f t="shared" si="21"/>
         <v>0.037582054886145654</v>
       </c>
     </row>
     <row r="28" ht="14.25">
-      <c r="A28" s="16" t="s">
+      <c r="A28" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="15">
+      <c r="B28" s="13">
         <v>0.35732421874999998</v>
       </c>
-      <c r="C28" s="15">
+      <c r="C28" s="13">
         <v>0.35732421874999998</v>
       </c>
-      <c r="D28" s="15">
+      <c r="D28" s="13">
         <v>0.39192382812499998</v>
       </c>
-      <c r="E28" s="15">
+      <c r="E28" s="13">
         <v>0.37104492187499999</v>
       </c>
-      <c r="F28" s="15">
+      <c r="F28" s="13">
         <v>0.36724283854166667</v>
       </c>
-      <c r="G28" s="16">
-        <f>AVERAGE(B28:F28)</f>
+      <c r="G28" s="14">
+        <f t="shared" si="20"/>
         <v>0.36897200520833329</v>
       </c>
-      <c r="H28" s="16">
-        <f>STDEV(B28:F28)</f>
+      <c r="H28" s="14">
+        <f t="shared" si="21"/>
         <v>0.014189917501732945</v>
       </c>
     </row>
     <row r="29" ht="14.25">
-      <c r="A29" s="16" t="s">
+      <c r="A29" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="B29" s="15">
+      <c r="B29" s="13">
         <v>0.27944010416666665</v>
       </c>
-      <c r="C29" s="15">
+      <c r="C29" s="13">
         <v>0.27944010416666665</v>
       </c>
-      <c r="D29" s="15">
+      <c r="D29" s="13">
         <v>0.40939127604166664</v>
       </c>
-      <c r="E29" s="15">
+      <c r="E29" s="13">
         <v>0.36391276041666665</v>
       </c>
-      <c r="F29" s="15">
+      <c r="F29" s="13">
         <v>0.36564453125000002</v>
       </c>
-      <c r="G29" s="16">
-        <f>AVERAGE(B29:F29)</f>
+      <c r="G29" s="14">
+        <f t="shared" si="20"/>
         <v>0.33956575520833338</v>
       </c>
-      <c r="H29" s="16">
-        <f>STDEV(B29:F29)</f>
+      <c r="H29" s="14">
+        <f t="shared" si="21"/>
         <v>0.057833101266620716</v>
       </c>
     </row>
     <row r="30" ht="14.25">
-      <c r="A30" s="16" t="s">
+      <c r="A30" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="B30" s="15">
+      <c r="B30" s="13">
         <v>0.33397135416666668</v>
       </c>
-      <c r="C30" s="15">
+      <c r="C30" s="13">
         <v>0.33397135416666668</v>
       </c>
-      <c r="D30" s="15">
+      <c r="D30" s="13">
         <v>0.40951822916666669</v>
       </c>
-      <c r="E30" s="15">
+      <c r="E30" s="13">
         <v>0.37071289062500001</v>
       </c>
-      <c r="F30" s="15">
+      <c r="F30" s="13">
         <v>0.36637369791666669</v>
       </c>
-      <c r="G30" s="16">
-        <f>AVERAGE(B30:F30)</f>
+      <c r="G30" s="14">
+        <f t="shared" si="20"/>
         <v>0.36290950520833343</v>
       </c>
-      <c r="H30" s="16">
-        <f>STDEV(B30:F30)</f>
+      <c r="H30" s="14">
+        <f t="shared" si="21"/>
         <v>0.031305350083996264</v>
       </c>
     </row>
@@ -3130,295 +3127,295 @@
       <c r="H1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="11"/>
+      <c r="I1" s="9"/>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="8">
         <v>0.20133789062499999</v>
       </c>
-      <c r="C2" s="10">
-        <f t="shared" ref="C2:C9" si="14">100*B2</f>
+      <c r="C2" s="8">
+        <f t="shared" ref="C2:C9" si="22">100*B2</f>
         <v>20.1337890625</v>
       </c>
-      <c r="D2" s="10">
-        <f t="shared" ref="D2:D9" si="15">ABS(C2/media5*100-100)</f>
+      <c r="D2" s="8">
+        <f t="shared" ref="D2:D9" si="23">ABS(C2/media5*100-100)</f>
         <v>22.173608161894691</v>
       </c>
-      <c r="E2" s="10">
-        <f t="shared" ref="E2:E9" si="16">ABS(C2/porosidade5*100-100)</f>
+      <c r="E2" s="8">
+        <f t="shared" ref="E2:E9" si="24">ABS(C2/porosidade5*100-100)</f>
         <v>23.153476860687022</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="8">
         <v>9.26971435546875</v>
       </c>
-      <c r="G2" s="11">
+      <c r="G2" s="9">
         <v>3022</v>
       </c>
-      <c r="H2" s="11">
+      <c r="H2" s="9">
         <v>3948</v>
       </c>
     </row>
     <row r="3" ht="14.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="8">
         <v>0.19438476562500001</v>
       </c>
-      <c r="C3" s="10">
-        <f t="shared" si="14"/>
+      <c r="C3" s="8">
+        <f t="shared" si="22"/>
         <v>19.4384765625</v>
       </c>
-      <c r="D3" s="10">
-        <f t="shared" si="15"/>
+      <c r="D3" s="8">
+        <f t="shared" si="23"/>
         <v>17.95439057392025</v>
       </c>
-      <c r="E3" s="10">
-        <f t="shared" si="16"/>
+      <c r="E3" s="8">
+        <f t="shared" si="24"/>
         <v>25.807341364503813</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="8">
         <v>9.1662406921386719</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="9">
         <v>5921</v>
       </c>
-      <c r="H3" s="11">
+      <c r="H3" s="9">
         <v>6761</v>
       </c>
     </row>
     <row r="4" ht="14.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="8">
         <v>0.16281901041666666</v>
       </c>
-      <c r="C4" s="10">
-        <f t="shared" si="14"/>
+      <c r="C4" s="8">
+        <f t="shared" si="22"/>
         <v>16.281901041666664</v>
       </c>
-      <c r="D4" s="10">
-        <f t="shared" si="15"/>
+      <c r="D4" s="8">
+        <f t="shared" si="23"/>
         <v>1.1999881482652199</v>
       </c>
-      <c r="E4" s="10">
-        <f t="shared" si="16"/>
+      <c r="E4" s="8">
+        <f t="shared" si="24"/>
         <v>37.855339535623422</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="8">
         <v>9.1207027435302734</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="9">
         <v>3024</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="9">
         <v>4209</v>
       </c>
     </row>
     <row r="5" ht="14.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="8">
         <v>0.16997721354166667</v>
       </c>
-      <c r="C5" s="10">
-        <f t="shared" si="14"/>
+      <c r="C5" s="8">
+        <f t="shared" si="22"/>
         <v>16.997721354166668</v>
       </c>
-      <c r="D5" s="10">
-        <f t="shared" si="15"/>
+      <c r="D5" s="8">
+        <f t="shared" si="23"/>
         <v>3.1436726550848846</v>
       </c>
-      <c r="E5" s="10">
-        <f t="shared" si="16"/>
+      <c r="E5" s="8">
+        <f t="shared" si="24"/>
         <v>35.123200938295156</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="8">
         <v>8.9459419250488281</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="9">
         <v>1900</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="9">
         <v>2963</v>
       </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="8">
         <v>0.22072916666666667</v>
       </c>
-      <c r="C6" s="10">
-        <f t="shared" si="14"/>
+      <c r="C6" s="8">
+        <f t="shared" si="22"/>
         <v>22.072916666666668</v>
       </c>
-      <c r="D6" s="10">
-        <f t="shared" si="15"/>
+      <c r="D6" s="8">
+        <f t="shared" si="23"/>
         <v>33.940405526858996</v>
       </c>
-      <c r="E6" s="10">
-        <f t="shared" si="16"/>
+      <c r="E6" s="8">
+        <f t="shared" si="24"/>
         <v>15.752226463104321</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="8">
         <v>14.075279235839844</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="9">
         <v>3112</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="9">
         <v>4529</v>
       </c>
     </row>
     <row r="7" ht="14.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="8">
         <v>0.20756510416666665</v>
       </c>
-      <c r="C7" s="10">
-        <f t="shared" si="14"/>
+      <c r="C7" s="8">
+        <f t="shared" si="22"/>
         <v>20.756510416666664</v>
       </c>
-      <c r="D7" s="10">
-        <f t="shared" si="15"/>
+      <c r="D7" s="8">
+        <f t="shared" si="23"/>
         <v>25.952336273221974</v>
       </c>
-      <c r="E7" s="10">
-        <f t="shared" si="16"/>
+      <c r="E7" s="8">
+        <f t="shared" si="24"/>
         <v>20.776677798982192</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="8">
         <v>8.87298583984375</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="9">
         <v>2154</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="9">
         <v>3869</v>
       </c>
     </row>
     <row r="8" ht="14.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="8">
         <v>0.076256510416666673</v>
       </c>
-      <c r="C8" s="10">
-        <f t="shared" si="14"/>
+      <c r="C8" s="8">
+        <f t="shared" si="22"/>
         <v>7.625651041666667</v>
       </c>
-      <c r="D8" s="10">
-        <f t="shared" si="15"/>
+      <c r="D8" s="8">
+        <f t="shared" si="23"/>
         <v>53.726876771587442</v>
       </c>
-      <c r="E8" s="10">
-        <f t="shared" si="16"/>
+      <c r="E8" s="8">
+        <f t="shared" si="24"/>
         <v>70.89446167302799</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="8">
         <v>9.2041492462158203</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="9">
         <v>1253</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="9">
         <v>4356</v>
       </c>
     </row>
     <row r="9" ht="14.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="8">
         <v>0.10691080729166667</v>
       </c>
-      <c r="C9" s="10">
-        <f t="shared" si="14"/>
+      <c r="C9" s="8">
+        <f t="shared" si="22"/>
         <v>10.691080729166668</v>
       </c>
-      <c r="D9" s="10">
-        <f t="shared" si="15"/>
+      <c r="D9" s="8">
+        <f t="shared" si="23"/>
         <v>35.125579006627092</v>
       </c>
-      <c r="E9" s="10">
-        <f t="shared" si="16"/>
+      <c r="E9" s="8">
+        <f t="shared" si="24"/>
         <v>59.194348361959278</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="8">
         <v>9.0672969818115234</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="9">
         <v>3181</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="9">
         <v>5068</v>
       </c>
     </row>
     <row r="10" ht="14.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="8">
         <v>0.11185872395833334</v>
       </c>
-      <c r="C10" s="10">
-        <f t="shared" ref="C10:C11" si="17">100*B10</f>
+      <c r="C10" s="8">
+        <f t="shared" ref="C10:C11" si="25">100*B10</f>
         <v>11.185872395833334</v>
       </c>
-      <c r="D10" s="10">
-        <f t="shared" ref="D10:D11" si="18">ABS(C10/media5*100-100)</f>
+      <c r="D10" s="8">
+        <f t="shared" ref="D10:D11" si="26">ABS(C10/media5*100-100)</f>
         <v>32.123139524547909</v>
       </c>
-      <c r="E10" s="10">
-        <f t="shared" ref="E10:E11" si="19">ABS(C10/porosidade5*100-100)</f>
+      <c r="E10" s="8">
+        <f t="shared" ref="E10:E11" si="27">ABS(C10/porosidade5*100-100)</f>
         <v>57.305830550254448</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="8">
         <v>8.9812278747558594</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="9">
         <v>2178</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="9">
         <v>4468</v>
       </c>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="8">
         <v>0.19612630208333334</v>
       </c>
-      <c r="C11" s="10">
-        <f t="shared" si="17"/>
+      <c r="C11" s="8">
+        <f t="shared" si="25"/>
         <v>19.612630208333336</v>
       </c>
-      <c r="D11" s="10">
-        <f t="shared" si="18"/>
+      <c r="D11" s="8">
+        <f t="shared" si="26"/>
         <v>19.011170260046811</v>
       </c>
-      <c r="E11" s="10">
-        <f t="shared" si="19"/>
+      <c r="E11" s="8">
+        <f t="shared" si="27"/>
         <v>25.142632792620859</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="8">
         <v>9.5262527465820312</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="9">
         <v>3662</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="9">
         <v>5946</v>
       </c>
     </row>
@@ -3426,13 +3423,13 @@
       <c r="B13" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="7">
         <f>AVERAGE(C2:C11)</f>
         <v>16.479654947916668</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9">
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7">
         <f>AVERAGE(F2:F11)</f>
         <v>9.6229791641235352</v>
       </c>
@@ -3441,13 +3438,13 @@
       <c r="B14" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="8">
         <f>STDEV(C2:C11)</f>
         <v>4.9635508636796208</v>
       </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="10">
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="8">
         <f>STDEV(F2:F11)</f>
         <v>1.5753283574050787</v>
       </c>
@@ -3456,330 +3453,330 @@
       <c r="B16" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="8">
         <v>26.199999999999999</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="8">
         <f>ABS(C13/porosidade5*100-100)</f>
         <v>37.100553633905839</v>
       </c>
-      <c r="E16" s="11"/>
+      <c r="E16" s="9"/>
     </row>
     <row r="19" ht="14.25">
-      <c r="A19" s="26" t="s">
+      <c r="A19" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="29"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="26"/>
     </row>
     <row r="20" ht="14.25">
-      <c r="A20" s="24"/>
-      <c r="B20" s="25" t="s">
+      <c r="A20" s="20"/>
+      <c r="B20" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="25" t="s">
+      <c r="C20" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="25" t="s">
+      <c r="D20" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="25" t="s">
+      <c r="E20" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="25" t="s">
+      <c r="F20" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="G20" s="25" t="s">
+      <c r="G20" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="21" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="21" ht="14.25">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="16">
+      <c r="B21" s="14">
         <v>0.20133789062499999</v>
       </c>
-      <c r="C21" s="15">
+      <c r="C21" s="13">
         <v>0.20133789062499999</v>
       </c>
-      <c r="D21" s="15">
+      <c r="D21" s="13">
         <v>0.20133789062499999</v>
       </c>
-      <c r="E21" s="15">
+      <c r="E21" s="13">
         <v>0.16134765625</v>
       </c>
-      <c r="F21" s="15">
+      <c r="F21" s="13">
         <v>0.2123135015615</v>
       </c>
-      <c r="G21" s="16">
-        <f>AVERAGE(B21:F21)</f>
+      <c r="G21" s="14">
+        <f t="shared" ref="G21:G30" si="28">AVERAGE(B21:F21)</f>
         <v>0.19553496593729999</v>
       </c>
-      <c r="H21" s="16">
-        <f>STDEV(B21:F21)</f>
+      <c r="H21" s="14">
+        <f t="shared" ref="H21:H30" si="29">STDEV(B21:F21)</f>
         <v>0.01969335678687904</v>
       </c>
     </row>
     <row r="22" ht="14.25">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="16">
+      <c r="B22" s="14">
         <v>0.19438476562500001</v>
       </c>
-      <c r="C22" s="15">
+      <c r="C22" s="13">
         <v>0.19438476562500001</v>
       </c>
-      <c r="D22" s="15">
+      <c r="D22" s="13">
         <v>0.19438476562500001</v>
       </c>
-      <c r="E22" s="15">
+      <c r="E22" s="13">
         <v>0.15660156250000001</v>
       </c>
-      <c r="F22" s="15">
+      <c r="F22" s="13">
         <v>0.20051456021500003</v>
       </c>
-      <c r="G22" s="16">
-        <f>AVERAGE(B22:F22)</f>
+      <c r="G22" s="14">
+        <f t="shared" si="28"/>
         <v>0.18805408391800002</v>
       </c>
-      <c r="H22" s="16">
-        <f>STDEV(B22:F22)</f>
+      <c r="H22" s="14">
+        <f t="shared" si="29"/>
         <v>0.01778171227500238</v>
       </c>
     </row>
     <row r="23" ht="14.25">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="16">
+      <c r="B23" s="14">
         <v>0.16281901041666666</v>
       </c>
-      <c r="C23" s="15">
+      <c r="C23" s="13">
         <v>0.16281901041666666</v>
       </c>
-      <c r="D23" s="15">
+      <c r="D23" s="13">
         <v>0.16281901041666666</v>
       </c>
-      <c r="E23" s="15">
+      <c r="E23" s="13">
         <v>0.15272786458333334</v>
       </c>
-      <c r="F23" s="15">
+      <c r="F23" s="13">
         <v>0.20057810499999998</v>
       </c>
-      <c r="G23" s="16">
-        <f>AVERAGE(B23:F23)</f>
+      <c r="G23" s="14">
+        <f t="shared" si="28"/>
         <v>0.16835260016666664</v>
       </c>
-      <c r="H23" s="16">
-        <f>STDEV(B23:F23)</f>
+      <c r="H23" s="14">
+        <f t="shared" si="29"/>
         <v>0.018536972314648546</v>
       </c>
     </row>
     <row r="24" ht="14.25">
-      <c r="A24" s="16" t="s">
+      <c r="A24" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="16">
+      <c r="B24" s="14">
         <v>0.16997721354166667</v>
       </c>
-      <c r="C24" s="15">
+      <c r="C24" s="13">
         <v>0.16997721354166667</v>
       </c>
-      <c r="D24" s="15">
+      <c r="D24" s="13">
         <v>0.16997721354166667</v>
       </c>
-      <c r="E24" s="15">
+      <c r="E24" s="13">
         <v>0.115068359375</v>
       </c>
-      <c r="F24" s="15">
+      <c r="F24" s="13">
         <v>0.1615840841</v>
       </c>
-      <c r="G24" s="16">
-        <f>AVERAGE(B24:F24)</f>
+      <c r="G24" s="14">
+        <f t="shared" si="28"/>
         <v>0.15731681682000004</v>
       </c>
-      <c r="H24" s="16">
-        <f>STDEV(B24:F24)</f>
+      <c r="H24" s="14">
+        <f t="shared" si="29"/>
         <v>0.023895599291349125</v>
       </c>
     </row>
     <row r="25" ht="14.25">
-      <c r="A25" s="16" t="s">
+      <c r="A25" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="16">
+      <c r="B25" s="14">
         <v>0.22072916666666667</v>
       </c>
-      <c r="C25" s="15">
+      <c r="C25" s="13">
         <v>0.22072916666666667</v>
       </c>
-      <c r="D25" s="15">
+      <c r="D25" s="13">
         <v>0.22072916666666667</v>
       </c>
-      <c r="E25" s="15">
+      <c r="E25" s="13">
         <v>0.17810872395833333</v>
       </c>
-      <c r="F25" s="15">
+      <c r="F25" s="13">
         <v>0.22084218115609999</v>
       </c>
-      <c r="G25" s="16">
-        <f>AVERAGE(B25:F25)</f>
+      <c r="G25" s="14">
+        <f t="shared" si="28"/>
         <v>0.21222768102288664</v>
       </c>
-      <c r="H25" s="16">
-        <f>STDEV(B25:F25)</f>
+      <c r="H25" s="14">
+        <f t="shared" si="29"/>
         <v>0.019073139608964222</v>
       </c>
     </row>
     <row r="26" ht="14.25">
-      <c r="A26" s="16" t="s">
+      <c r="A26" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="16">
+      <c r="B26" s="14">
         <v>0.20756510416666665</v>
       </c>
-      <c r="C26" s="15">
+      <c r="C26" s="13">
         <v>0.20756510416666665</v>
       </c>
-      <c r="D26" s="15">
+      <c r="D26" s="13">
         <v>0.20756510416666665</v>
       </c>
-      <c r="E26" s="15">
+      <c r="E26" s="13">
         <v>0.19865234374999999</v>
       </c>
-      <c r="F26" s="15">
+      <c r="F26" s="13">
         <v>0.2105478978101</v>
       </c>
-      <c r="G26" s="16">
-        <f>AVERAGE(B26:F26)</f>
+      <c r="G26" s="14">
+        <f t="shared" si="28"/>
         <v>0.20637911081202001</v>
       </c>
-      <c r="H26" s="16">
-        <f>STDEV(B26:F26)</f>
+      <c r="H26" s="14">
+        <f t="shared" si="29"/>
         <v>0.0045083659727742902</v>
       </c>
     </row>
     <row r="27" ht="14.25">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="16">
+      <c r="B27" s="14">
         <v>0.076256510416666673</v>
       </c>
-      <c r="C27" s="15">
+      <c r="C27" s="13">
         <v>0.076256510416666673</v>
       </c>
-      <c r="D27" s="15">
+      <c r="D27" s="13">
         <v>0.076256510416666673</v>
       </c>
-      <c r="E27" s="15">
+      <c r="E27" s="13">
         <v>0.086940104166666671</v>
       </c>
-      <c r="F27" s="15">
+      <c r="F27" s="13">
         <v>0.100548784154989</v>
       </c>
-      <c r="G27" s="16">
-        <f>AVERAGE(B27:F27)</f>
+      <c r="G27" s="14">
+        <f t="shared" si="28"/>
         <v>0.083251683914331132</v>
       </c>
-      <c r="H27" s="16">
-        <f>STDEV(B27:F27)</f>
+      <c r="H27" s="14">
+        <f t="shared" si="29"/>
         <v>0.010719042371878271</v>
       </c>
     </row>
     <row r="28" ht="14.25">
-      <c r="A28" s="16" t="s">
+      <c r="A28" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="16">
+      <c r="B28" s="14">
         <v>0.10691080729166667</v>
       </c>
-      <c r="C28" s="15">
+      <c r="C28" s="13">
         <v>0.10691080729166667</v>
       </c>
-      <c r="D28" s="15">
+      <c r="D28" s="13">
         <v>0.10691080729166667</v>
       </c>
-      <c r="E28" s="15">
+      <c r="E28" s="13">
         <v>0.10408203125</v>
       </c>
-      <c r="F28" s="23">
+      <c r="F28" s="13">
         <v>0.1040487871</v>
       </c>
-      <c r="G28" s="16">
-        <f>AVERAGE(B28:F28)</f>
+      <c r="G28" s="14">
+        <f t="shared" si="28"/>
         <v>0.105772648045</v>
       </c>
-      <c r="H28" s="16">
-        <f>STDEV(B28:F28)</f>
+      <c r="H28" s="14">
+        <f t="shared" si="29"/>
         <v>0.0015585330536718597</v>
       </c>
     </row>
     <row r="29" ht="14.25">
-      <c r="A29" s="16" t="s">
+      <c r="A29" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="B29" s="16">
+      <c r="B29" s="14">
         <v>0.11185872395833334</v>
       </c>
-      <c r="C29" s="15">
+      <c r="C29" s="13">
         <v>0.11185872395833334</v>
       </c>
-      <c r="D29" s="15">
+      <c r="D29" s="13">
         <v>0.11185872395833334</v>
       </c>
-      <c r="E29" s="15">
+      <c r="E29" s="13">
         <v>0.11831705729166667</v>
       </c>
-      <c r="F29" s="15">
+      <c r="F29" s="13">
         <v>0.1105489781</v>
       </c>
-      <c r="G29" s="16">
-        <f>AVERAGE(B29:F29)</f>
+      <c r="G29" s="14">
+        <f t="shared" si="28"/>
         <v>0.11288844145333332</v>
       </c>
-      <c r="H29" s="16">
-        <f>STDEV(B29:F29)</f>
+      <c r="H29" s="14">
+        <f t="shared" si="29"/>
         <v>0.0030872282495921959</v>
       </c>
     </row>
     <row r="30" ht="14.25">
-      <c r="A30" s="16" t="s">
+      <c r="A30" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="B30" s="16">
+      <c r="B30" s="14">
         <v>0.19612630208333334</v>
       </c>
-      <c r="C30" s="15">
+      <c r="C30" s="13">
         <v>0.19612630208333334</v>
       </c>
-      <c r="D30" s="15">
+      <c r="D30" s="13">
         <v>0.19612630208333334</v>
       </c>
-      <c r="E30" s="15">
+      <c r="E30" s="13">
         <v>0.16398763020833335</v>
       </c>
-      <c r="F30" s="15">
+      <c r="F30" s="13">
         <v>0.200547481548978</v>
       </c>
-      <c r="G30" s="16">
-        <f>AVERAGE(B30:F30)</f>
+      <c r="G30" s="14">
+        <f t="shared" si="28"/>
         <v>0.19058280360146229</v>
       </c>
-      <c r="H30" s="16">
-        <f>STDEV(B30:F30)</f>
+      <c r="H30" s="14">
+        <f t="shared" si="29"/>
         <v>0.014989906442868645</v>
       </c>
     </row>
@@ -3816,35 +3813,35 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" s="30"/>
-      <c r="B1" s="31" t="s">
+      <c r="A1" s="27"/>
+      <c r="B1" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31" t="s">
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31" t="s">
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31" t="s">
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31" t="s">
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2" s="30"/>
+      <c r="A2" s="27"/>
       <c r="B2" s="2" t="s">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
fix typos, figures references and tables
</commit_message>
<xml_diff>
--- a/resultados/resultados.xlsx
+++ b/resultados/resultados.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Berea200" sheetId="1" state="visible" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>Imagem</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>Solido</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
   <si>
     <t>I31</t>
@@ -347,7 +350,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="2" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -376,6 +379,9 @@
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1199,10 +1205,13 @@
       <c r="G1" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="2" ht="14.25">
       <c r="A2" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B2" s="7">
         <v>0.22181640624999999</v>
@@ -1224,10 +1233,14 @@
       <c r="G2">
         <v>4457</v>
       </c>
+      <c r="H2">
+        <f>F2+G2</f>
+        <v>8482</v>
+      </c>
     </row>
     <row r="3" ht="14.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" s="7">
         <v>0.23427408854166668</v>
@@ -1249,10 +1262,14 @@
       <c r="G3">
         <v>5604</v>
       </c>
+      <c r="H3">
+        <f>F3+G3</f>
+        <v>9971</v>
+      </c>
     </row>
     <row r="4" ht="14.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" s="7">
         <v>0.22600911458333334</v>
@@ -1274,10 +1291,14 @@
       <c r="G4">
         <v>4710</v>
       </c>
+      <c r="H4">
+        <f>F4+G4</f>
+        <v>7848</v>
+      </c>
     </row>
     <row r="5" ht="14.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" s="7">
         <v>0.34716471354166667</v>
@@ -1299,10 +1320,14 @@
       <c r="G5">
         <v>4199</v>
       </c>
+      <c r="H5">
+        <f>F5+G5</f>
+        <v>8047</v>
+      </c>
     </row>
     <row r="6" ht="14.25">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B6" s="7">
         <v>0.24533203125</v>
@@ -1324,10 +1349,14 @@
       <c r="G6">
         <v>4323</v>
       </c>
+      <c r="H6">
+        <f>F6+G6</f>
+        <v>7565</v>
+      </c>
     </row>
     <row r="7" ht="14.25">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B7" s="7">
         <v>0.21280924479166666</v>
@@ -1349,10 +1378,14 @@
       <c r="G7">
         <v>5269</v>
       </c>
+      <c r="H7">
+        <f>F7+G7</f>
+        <v>9757</v>
+      </c>
     </row>
     <row r="8" ht="14.25">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" s="7">
         <v>0.144560546875</v>
@@ -1373,6 +1406,10 @@
       </c>
       <c r="G8">
         <v>4611</v>
+      </c>
+      <c r="H8">
+        <f>F8+G8</f>
+        <v>8304</v>
       </c>
     </row>
     <row r="9" ht="14.25"/>
@@ -1445,7 +1482,7 @@
     </row>
     <row r="15" ht="14.25">
       <c r="A15" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B15" s="13">
         <v>0.22181640624999999</v>
@@ -1473,7 +1510,7 @@
     </row>
     <row r="16" ht="14.25">
       <c r="A16" s="15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B16" s="13">
         <v>0.23427408854166668</v>
@@ -1501,7 +1538,7 @@
     </row>
     <row r="17" ht="14.25">
       <c r="A17" s="15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B17" s="13">
         <v>0.22600911458333334</v>
@@ -1529,7 +1566,7 @@
     </row>
     <row r="18" ht="14.25">
       <c r="A18" s="15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B18" s="13">
         <v>0.34716471354166667</v>
@@ -1557,7 +1594,7 @@
     </row>
     <row r="19" ht="14.25">
       <c r="A19" s="15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B19" s="13">
         <v>0.24533203125</v>
@@ -1585,7 +1622,7 @@
     </row>
     <row r="20" ht="14.25">
       <c r="A20" s="15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B20" s="13">
         <v>0.21280924479166666</v>
@@ -1613,7 +1650,7 @@
     </row>
     <row r="21" ht="14.25">
       <c r="A21" s="15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B21" s="13">
         <v>0.144560546875</v>
@@ -1690,7 +1727,7 @@
         <v>14</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>15</v>
@@ -1701,11 +1738,13 @@
       <c r="H1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="9"/>
+      <c r="I1" s="16" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="2" ht="14.25">
       <c r="A2" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B2" s="7">
         <v>0.24501953125000001</v>
@@ -1731,10 +1770,14 @@
       <c r="H2">
         <v>2382</v>
       </c>
+      <c r="I2">
+        <f>G2+H2</f>
+        <v>3592</v>
+      </c>
     </row>
     <row r="3" ht="14.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B3" s="7">
         <v>0.062360026041666669</v>
@@ -1760,10 +1803,14 @@
       <c r="H3">
         <v>2745</v>
       </c>
+      <c r="I3">
+        <f>G3+H3</f>
+        <v>4663</v>
+      </c>
     </row>
     <row r="4" ht="14.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B4" s="7">
         <v>0.20591471354166666</v>
@@ -1789,10 +1836,14 @@
       <c r="H4">
         <v>2557</v>
       </c>
+      <c r="I4">
+        <f>G4+H4</f>
+        <v>4290</v>
+      </c>
     </row>
     <row r="5" ht="14.25">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B5" s="7">
         <v>0.093710937499999994</v>
@@ -1818,10 +1869,14 @@
       <c r="H5">
         <v>2113</v>
       </c>
+      <c r="I5">
+        <f>G5+H5</f>
+        <v>3455</v>
+      </c>
     </row>
     <row r="6" ht="14.25">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B6" s="7">
         <v>0.24616536458333332</v>
@@ -1847,10 +1902,14 @@
       <c r="H6">
         <v>2279</v>
       </c>
+      <c r="I6">
+        <f>G6+H6</f>
+        <v>3820</v>
+      </c>
     </row>
     <row r="7" ht="14.25">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B7" s="7">
         <v>0.37842447916666666</v>
@@ -1876,10 +1935,14 @@
       <c r="H7">
         <v>1765</v>
       </c>
+      <c r="I7">
+        <f>G7+H7</f>
+        <v>3142</v>
+      </c>
     </row>
     <row r="8" ht="14.25">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B8" s="7">
         <v>0.30426757812499999</v>
@@ -1905,10 +1968,14 @@
       <c r="H8">
         <v>2544</v>
       </c>
+      <c r="I8">
+        <f>G8+H8</f>
+        <v>3930</v>
+      </c>
     </row>
     <row r="9" ht="14.25">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B9" s="7">
         <v>0.33873046875000001</v>
@@ -1934,10 +2001,14 @@
       <c r="H9">
         <v>1629</v>
       </c>
+      <c r="I9">
+        <f>G9+H9</f>
+        <v>3113</v>
+      </c>
     </row>
     <row r="10" ht="14.25">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B10" s="7">
         <v>0.22583658854166666</v>
@@ -1963,10 +2034,14 @@
       <c r="H10">
         <v>2137</v>
       </c>
+      <c r="I10">
+        <f>G10+H10</f>
+        <v>3783</v>
+      </c>
     </row>
     <row r="11" ht="14.25">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B11" s="7">
         <v>0.27026041666666667</v>
@@ -1991,6 +2066,10 @@
       </c>
       <c r="H11">
         <v>2052</v>
+      </c>
+      <c r="I11">
+        <f>G11+H11</f>
+        <v>3231</v>
       </c>
     </row>
     <row r="13" ht="14.25">
@@ -2025,7 +2104,7 @@
     </row>
     <row r="16" ht="14.25">
       <c r="B16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C16" s="8">
         <v>14.800000000000001</v>
@@ -2036,18 +2115,18 @@
       </c>
     </row>
     <row r="18" ht="14.25">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="20"/>
     </row>
     <row r="19" ht="14.25">
       <c r="A19" s="10"/>
@@ -2075,7 +2154,7 @@
     </row>
     <row r="20" ht="14.25">
       <c r="A20" s="12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B20" s="13">
         <v>0.24501953125000001</v>
@@ -2103,7 +2182,7 @@
     </row>
     <row r="21" ht="14.25">
       <c r="A21" s="15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B21" s="13">
         <v>0.062360026041666669</v>
@@ -2131,7 +2210,7 @@
     </row>
     <row r="22" ht="14.25">
       <c r="A22" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B22" s="13">
         <v>0.20591471354166666</v>
@@ -2159,7 +2238,7 @@
     </row>
     <row r="23" ht="14.25">
       <c r="A23" s="15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B23" s="13">
         <v>0.093710937499999994</v>
@@ -2187,7 +2266,7 @@
     </row>
     <row r="24" ht="14.25">
       <c r="A24" s="15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B24" s="13">
         <v>0.24616536458333332</v>
@@ -2215,7 +2294,7 @@
     </row>
     <row r="25" ht="14.25">
       <c r="A25" s="15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B25" s="13">
         <v>0.37842447916666666</v>
@@ -2243,7 +2322,7 @@
     </row>
     <row r="26" ht="14.25">
       <c r="A26" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B26" s="13">
         <v>0.30426757812499999</v>
@@ -2271,7 +2350,7 @@
     </row>
     <row r="27" ht="14.25">
       <c r="A27" s="12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B27" s="13">
         <v>0.33873046875000001</v>
@@ -2299,7 +2378,7 @@
     </row>
     <row r="28" ht="14.25">
       <c r="A28" s="12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B28" s="13">
         <v>0.22583658854166666</v>
@@ -2327,7 +2406,7 @@
     </row>
     <row r="29" ht="14.25">
       <c r="A29" s="12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B29" s="13">
         <v>0.27026041666666667</v>
@@ -2403,7 +2482,7 @@
         <v>14</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>15</v>
@@ -2414,11 +2493,13 @@
       <c r="H1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="9"/>
+      <c r="I1" s="16" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="2" ht="14.25">
       <c r="A2" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B2" s="8">
         <v>0.27605794270833334</v>
@@ -2444,10 +2525,14 @@
       <c r="H2" s="9">
         <v>2257</v>
       </c>
+      <c r="I2">
+        <f>G2+H2</f>
+        <v>4163</v>
+      </c>
     </row>
     <row r="3" ht="14.25">
       <c r="A3" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B3" s="8">
         <v>0.341064453125</v>
@@ -2473,10 +2558,14 @@
       <c r="H3" s="9">
         <v>2162</v>
       </c>
+      <c r="I3">
+        <f>G3+H3</f>
+        <v>3869</v>
+      </c>
     </row>
     <row r="4" ht="14.25">
       <c r="A4" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B4" s="8">
         <v>0.27746744791666667</v>
@@ -2502,10 +2591,14 @@
       <c r="H4" s="9">
         <v>2898</v>
       </c>
+      <c r="I4">
+        <f>G4+H4</f>
+        <v>5549</v>
+      </c>
     </row>
     <row r="5" ht="14.25">
       <c r="A5" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B5" s="8">
         <v>0.31875976562500002</v>
@@ -2531,10 +2624,14 @@
       <c r="H5" s="9">
         <v>3189</v>
       </c>
+      <c r="I5">
+        <f>G5+H5</f>
+        <v>5409</v>
+      </c>
     </row>
     <row r="6" ht="14.25">
       <c r="A6" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B6" s="8">
         <v>0.25666666666666665</v>
@@ -2560,10 +2657,14 @@
       <c r="H6" s="9">
         <v>2168</v>
       </c>
+      <c r="I6">
+        <f>G6+H6</f>
+        <v>4201</v>
+      </c>
     </row>
     <row r="7" ht="14.25">
       <c r="A7" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B7" s="8">
         <v>0.28517578124999998</v>
@@ -2589,10 +2690,14 @@
       <c r="H7" s="9">
         <v>2517</v>
       </c>
+      <c r="I7">
+        <f>G7+H7</f>
+        <v>5033</v>
+      </c>
     </row>
     <row r="8" ht="14.25">
       <c r="A8" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B8" s="8">
         <v>0.43480468750000001</v>
@@ -2618,10 +2723,14 @@
       <c r="H8" s="9">
         <v>2311</v>
       </c>
+      <c r="I8">
+        <f>G8+H8</f>
+        <v>5002</v>
+      </c>
     </row>
     <row r="9" ht="14.25">
       <c r="A9" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B9" s="8">
         <v>0.35732421874999998</v>
@@ -2647,10 +2756,14 @@
       <c r="H9" s="9">
         <v>2275</v>
       </c>
+      <c r="I9">
+        <f>G9+H9</f>
+        <v>4569</v>
+      </c>
     </row>
     <row r="10" ht="14.25">
       <c r="A10" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B10" s="8">
         <v>0.27944010416666665</v>
@@ -2676,10 +2789,14 @@
       <c r="H10" s="9">
         <v>3429</v>
       </c>
+      <c r="I10">
+        <f>G10+H10</f>
+        <v>6102</v>
+      </c>
     </row>
     <row r="11" ht="14.25">
       <c r="A11" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B11" s="8">
         <v>0.33397135416666668</v>
@@ -2704,6 +2821,10 @@
       </c>
       <c r="H11" s="9">
         <v>2426</v>
+      </c>
+      <c r="I11">
+        <f>G11+H11</f>
+        <v>4538</v>
       </c>
     </row>
     <row r="13" ht="14.25">
@@ -2738,7 +2859,7 @@
     </row>
     <row r="16" ht="14.25">
       <c r="B16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C16" s="7">
         <v>24</v>
@@ -2749,46 +2870,46 @@
       </c>
     </row>
     <row r="19" ht="14.25">
-      <c r="A19" s="20" t="s">
+      <c r="A19" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
     </row>
     <row r="20" ht="14.25">
-      <c r="A20" s="20"/>
-      <c r="B20" s="21" t="s">
+      <c r="A20" s="21"/>
+      <c r="B20" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="21" t="s">
+      <c r="D20" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="21" t="s">
+      <c r="E20" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="21" t="s">
+      <c r="F20" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="G20" s="21" t="s">
+      <c r="G20" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="H20" s="21" t="s">
+      <c r="H20" s="22" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="21" ht="14.25">
-      <c r="A21" s="22" t="s">
-        <v>37</v>
+      <c r="A21" s="23" t="s">
+        <v>38</v>
       </c>
       <c r="B21" s="13">
         <v>0.27605794270833334</v>
@@ -2815,8 +2936,8 @@
       </c>
     </row>
     <row r="22" ht="14.25">
-      <c r="A22" s="22" t="s">
-        <v>38</v>
+      <c r="A22" s="23" t="s">
+        <v>39</v>
       </c>
       <c r="B22" s="13">
         <v>0.341064453125</v>
@@ -2843,8 +2964,8 @@
       </c>
     </row>
     <row r="23" ht="14.25">
-      <c r="A23" s="22" t="s">
-        <v>39</v>
+      <c r="A23" s="23" t="s">
+        <v>40</v>
       </c>
       <c r="B23" s="13">
         <v>0.27746744791666667</v>
@@ -2871,8 +2992,8 @@
       </c>
     </row>
     <row r="24" ht="14.25">
-      <c r="A24" s="22" t="s">
-        <v>40</v>
+      <c r="A24" s="23" t="s">
+        <v>41</v>
       </c>
       <c r="B24" s="13">
         <v>0.31875976562500002</v>
@@ -2899,8 +3020,8 @@
       </c>
     </row>
     <row r="25" ht="14.25">
-      <c r="A25" s="22" t="s">
-        <v>41</v>
+      <c r="A25" s="23" t="s">
+        <v>42</v>
       </c>
       <c r="B25" s="13">
         <v>0.25666666666666665</v>
@@ -2927,8 +3048,8 @@
       </c>
     </row>
     <row r="26" ht="14.25">
-      <c r="A26" s="22" t="s">
-        <v>42</v>
+      <c r="A26" s="23" t="s">
+        <v>43</v>
       </c>
       <c r="B26" s="13">
         <v>0.28517578124999998</v>
@@ -2955,8 +3076,8 @@
       </c>
     </row>
     <row r="27" ht="14.25">
-      <c r="A27" s="22" t="s">
-        <v>43</v>
+      <c r="A27" s="23" t="s">
+        <v>44</v>
       </c>
       <c r="B27" s="13">
         <v>0.43480468750000001</v>
@@ -2983,8 +3104,8 @@
       </c>
     </row>
     <row r="28" ht="14.25">
-      <c r="A28" s="22" t="s">
-        <v>44</v>
+      <c r="A28" s="23" t="s">
+        <v>45</v>
       </c>
       <c r="B28" s="13">
         <v>0.35732421874999998</v>
@@ -3011,8 +3132,8 @@
       </c>
     </row>
     <row r="29" ht="14.25">
-      <c r="A29" s="22" t="s">
-        <v>45</v>
+      <c r="A29" s="23" t="s">
+        <v>46</v>
       </c>
       <c r="B29" s="13">
         <v>0.27944010416666665</v>
@@ -3039,8 +3160,8 @@
       </c>
     </row>
     <row r="30" ht="14.25">
-      <c r="A30" s="22" t="s">
-        <v>46</v>
+      <c r="A30" s="23" t="s">
+        <v>47</v>
       </c>
       <c r="B30" s="13">
         <v>0.33397135416666668</v>
@@ -3116,7 +3237,7 @@
         <v>14</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>15</v>
@@ -3131,7 +3252,7 @@
     </row>
     <row r="2" ht="14.25">
       <c r="A2" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B2" s="8">
         <v>0.20133789062499999</v>
@@ -3160,7 +3281,7 @@
     </row>
     <row r="3" ht="14.25">
       <c r="A3" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B3" s="8">
         <v>0.19438476562500001</v>
@@ -3189,7 +3310,7 @@
     </row>
     <row r="4" ht="14.25">
       <c r="A4" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B4" s="8">
         <v>0.16281901041666666</v>
@@ -3218,7 +3339,7 @@
     </row>
     <row r="5" ht="14.25">
       <c r="A5" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B5" s="8">
         <v>0.16997721354166667</v>
@@ -3247,7 +3368,7 @@
     </row>
     <row r="6" ht="14.25">
       <c r="A6" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B6" s="8">
         <v>0.22072916666666667</v>
@@ -3276,7 +3397,7 @@
     </row>
     <row r="7" ht="14.25">
       <c r="A7" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B7" s="8">
         <v>0.20756510416666665</v>
@@ -3305,7 +3426,7 @@
     </row>
     <row r="8" ht="14.25">
       <c r="A8" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B8" s="8">
         <v>0.076256510416666673</v>
@@ -3334,7 +3455,7 @@
     </row>
     <row r="9" ht="14.25">
       <c r="A9" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B9" s="8">
         <v>0.10691080729166667</v>
@@ -3363,7 +3484,7 @@
     </row>
     <row r="10" ht="14.25">
       <c r="A10" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B10" s="8">
         <v>0.11185872395833334</v>
@@ -3392,7 +3513,7 @@
     </row>
     <row r="11" ht="14.25">
       <c r="A11" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B11" s="8">
         <v>0.19612630208333334</v>
@@ -3451,7 +3572,7 @@
     </row>
     <row r="16" ht="14.25">
       <c r="B16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C16" s="8">
         <v>26.199999999999999</v>
@@ -3463,46 +3584,46 @@
       <c r="E16" s="9"/>
     </row>
     <row r="19" ht="14.25">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="27"/>
     </row>
     <row r="20" ht="14.25">
-      <c r="A20" s="20"/>
-      <c r="B20" s="21" t="s">
+      <c r="A20" s="21"/>
+      <c r="B20" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="21" t="s">
+      <c r="D20" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="21" t="s">
+      <c r="E20" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="21" t="s">
+      <c r="F20" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="G20" s="21" t="s">
+      <c r="G20" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="H20" s="21" t="s">
+      <c r="H20" s="22" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="21" ht="14.25">
-      <c r="A21" s="22" t="s">
-        <v>37</v>
+      <c r="A21" s="23" t="s">
+        <v>38</v>
       </c>
       <c r="B21" s="14">
         <v>0.20133789062499999</v>
@@ -3529,8 +3650,8 @@
       </c>
     </row>
     <row r="22" ht="14.25">
-      <c r="A22" s="22" t="s">
-        <v>38</v>
+      <c r="A22" s="23" t="s">
+        <v>39</v>
       </c>
       <c r="B22" s="14">
         <v>0.19438476562500001</v>
@@ -3557,8 +3678,8 @@
       </c>
     </row>
     <row r="23" ht="14.25">
-      <c r="A23" s="22" t="s">
-        <v>39</v>
+      <c r="A23" s="23" t="s">
+        <v>40</v>
       </c>
       <c r="B23" s="14">
         <v>0.16281901041666666</v>
@@ -3585,8 +3706,8 @@
       </c>
     </row>
     <row r="24" ht="14.25">
-      <c r="A24" s="22" t="s">
-        <v>40</v>
+      <c r="A24" s="23" t="s">
+        <v>41</v>
       </c>
       <c r="B24" s="14">
         <v>0.16997721354166667</v>
@@ -3613,8 +3734,8 @@
       </c>
     </row>
     <row r="25" ht="14.25">
-      <c r="A25" s="22" t="s">
-        <v>41</v>
+      <c r="A25" s="23" t="s">
+        <v>42</v>
       </c>
       <c r="B25" s="14">
         <v>0.22072916666666667</v>
@@ -3641,8 +3762,8 @@
       </c>
     </row>
     <row r="26" ht="14.25">
-      <c r="A26" s="22" t="s">
-        <v>42</v>
+      <c r="A26" s="23" t="s">
+        <v>43</v>
       </c>
       <c r="B26" s="14">
         <v>0.20756510416666665</v>
@@ -3669,8 +3790,8 @@
       </c>
     </row>
     <row r="27" ht="14.25">
-      <c r="A27" s="22" t="s">
-        <v>43</v>
+      <c r="A27" s="23" t="s">
+        <v>44</v>
       </c>
       <c r="B27" s="14">
         <v>0.076256510416666673</v>
@@ -3697,8 +3818,8 @@
       </c>
     </row>
     <row r="28" ht="14.25">
-      <c r="A28" s="22" t="s">
-        <v>44</v>
+      <c r="A28" s="23" t="s">
+        <v>45</v>
       </c>
       <c r="B28" s="14">
         <v>0.10691080729166667</v>
@@ -3725,8 +3846,8 @@
       </c>
     </row>
     <row r="29" ht="14.25">
-      <c r="A29" s="22" t="s">
-        <v>45</v>
+      <c r="A29" s="23" t="s">
+        <v>46</v>
       </c>
       <c r="B29" s="14">
         <v>0.11185872395833334</v>
@@ -3753,8 +3874,8 @@
       </c>
     </row>
     <row r="30" ht="14.25">
-      <c r="A30" s="22" t="s">
-        <v>46</v>
+      <c r="A30" s="23" t="s">
+        <v>47</v>
       </c>
       <c r="B30" s="14">
         <v>0.19612630208333334</v>
@@ -3813,76 +3934,76 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" s="27"/>
-      <c r="B1" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28" t="s">
+      <c r="A1" s="28"/>
+      <c r="B1" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28" t="s">
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28" t="s">
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28" t="s">
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2" s="27"/>
+      <c r="A2" s="28"/>
       <c r="B2" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>1</v>
@@ -3890,7 +4011,7 @@
     </row>
     <row r="3" ht="14.25">
       <c r="A3" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B3">
         <v>3147</v>
@@ -3940,7 +4061,7 @@
     </row>
     <row r="4" ht="14.25">
       <c r="A4" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B4">
         <v>3259</v>
@@ -3990,7 +4111,7 @@
     </row>
     <row r="5" ht="14.25">
       <c r="A5" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B5">
         <v>3895</v>
@@ -4040,7 +4161,7 @@
     </row>
     <row r="6" ht="14.25">
       <c r="A6" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B6">
         <v>2087</v>

</xml_diff>

<commit_message>
compare results with rego2010
</commit_message>
<xml_diff>
--- a/resultados/resultados.xlsx
+++ b/resultados/resultados.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Berea200" sheetId="1" state="visible" r:id="rId1"/>
@@ -3248,7 +3248,9 @@
       <c r="H1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="9"/>
+      <c r="I1" s="16" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="2" ht="14.25">
       <c r="A2" s="9" t="s">
@@ -3278,6 +3280,10 @@
       <c r="H2" s="9">
         <v>3948</v>
       </c>
+      <c r="I2">
+        <f>G2+H2</f>
+        <v>6970</v>
+      </c>
     </row>
     <row r="3" ht="14.25">
       <c r="A3" s="9" t="s">
@@ -3307,6 +3313,10 @@
       <c r="H3" s="9">
         <v>6761</v>
       </c>
+      <c r="I3">
+        <f>G3+H3</f>
+        <v>12682</v>
+      </c>
     </row>
     <row r="4" ht="14.25">
       <c r="A4" s="9" t="s">
@@ -3336,6 +3346,10 @@
       <c r="H4" s="9">
         <v>4209</v>
       </c>
+      <c r="I4">
+        <f>G4+H4</f>
+        <v>7233</v>
+      </c>
     </row>
     <row r="5" ht="14.25">
       <c r="A5" s="9" t="s">
@@ -3365,6 +3379,10 @@
       <c r="H5" s="9">
         <v>2963</v>
       </c>
+      <c r="I5">
+        <f>G5+H5</f>
+        <v>4863</v>
+      </c>
     </row>
     <row r="6" ht="14.25">
       <c r="A6" s="9" t="s">
@@ -3394,6 +3412,10 @@
       <c r="H6" s="9">
         <v>4529</v>
       </c>
+      <c r="I6">
+        <f>G6+H6</f>
+        <v>7641</v>
+      </c>
     </row>
     <row r="7" ht="14.25">
       <c r="A7" s="9" t="s">
@@ -3423,6 +3445,10 @@
       <c r="H7" s="9">
         <v>3869</v>
       </c>
+      <c r="I7">
+        <f>G7+H7</f>
+        <v>6023</v>
+      </c>
     </row>
     <row r="8" ht="14.25">
       <c r="A8" s="9" t="s">
@@ -3452,6 +3478,10 @@
       <c r="H8" s="9">
         <v>4356</v>
       </c>
+      <c r="I8">
+        <f>G8+H8</f>
+        <v>5609</v>
+      </c>
     </row>
     <row r="9" ht="14.25">
       <c r="A9" s="9" t="s">
@@ -3481,6 +3511,10 @@
       <c r="H9" s="9">
         <v>5068</v>
       </c>
+      <c r="I9">
+        <f>G9+H9</f>
+        <v>8249</v>
+      </c>
     </row>
     <row r="10" ht="14.25">
       <c r="A10" s="9" t="s">
@@ -3510,6 +3544,10 @@
       <c r="H10" s="9">
         <v>4468</v>
       </c>
+      <c r="I10">
+        <f>G10+H10</f>
+        <v>6646</v>
+      </c>
     </row>
     <row r="11" ht="14.25">
       <c r="A11" s="9" t="s">
@@ -3538,6 +3576,10 @@
       </c>
       <c r="H11" s="9">
         <v>5946</v>
+      </c>
+      <c r="I11">
+        <f>G11+H11</f>
+        <v>9608</v>
       </c>
     </row>
     <row r="13" ht="14.25">

</xml_diff>